<commit_message>
saving current branch to make etf object class
</commit_message>
<xml_diff>
--- a/src/testPlatform.xlsx
+++ b/src/testPlatform.xlsx
@@ -10948,8 +10948,9 @@
     </row>
     <row r="2" ht="21" customFormat="1" customHeight="1" s="1638">
       <c r="A2" s="24" t="n"/>
-      <c r="B2" s="1641" t="n">
-        <v>45078.98496527778</v>
+      <c r="B2" s="1641">
+        <f>NOW()</f>
+        <v/>
       </c>
       <c r="C2" s="26" t="inlineStr">
         <is>
@@ -11020,8 +11021,9 @@
     </row>
     <row r="3" ht="18" customFormat="1" customHeight="1" s="1638">
       <c r="A3" s="52" t="n"/>
-      <c r="B3" s="1642" t="n">
-        <v>45078.98496527778</v>
+      <c r="B3" s="1642">
+        <f>NOW()</f>
+        <v/>
       </c>
       <c r="C3" s="1643" t="n">
         <v>100000</v>
@@ -11031,8 +11033,9 @@
       </c>
       <c r="E3" s="56" t="n"/>
       <c r="F3" s="57" t="n"/>
-      <c r="G3" s="1644" t="n">
-        <v>1000</v>
+      <c r="G3" s="1644">
+        <f>C3*D3</f>
+        <v/>
       </c>
       <c r="H3" s="59" t="inlineStr">
         <is>
@@ -11370,7 +11373,7 @@
       <c r="D6" s="137" t="n"/>
       <c r="E6" s="138" t="inlineStr">
         <is>
-          <t>06/19</t>
+          <t>06/22</t>
         </is>
       </c>
       <c r="F6" s="139" t="inlineStr">
@@ -11379,7 +11382,7 @@
         </is>
       </c>
       <c r="G6" s="1646" t="n">
-        <v>91.91</v>
+        <v>-1</v>
       </c>
       <c r="H6" s="1647" t="n">
         <v>91.54000000000001</v>
@@ -11399,66 +11402,74 @@
       <c r="M6" s="1648" t="n">
         <v>91.93000000000001</v>
       </c>
-      <c r="N6" s="143" t="inlineStr">
-        <is>
-          <t>HOLD</t>
-        </is>
-      </c>
-      <c r="O6" s="144" t="n">
-        <v>0</v>
-      </c>
-      <c r="P6" s="1649" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q6" s="1650" t="n">
-        <v>0.06</v>
-      </c>
-      <c r="R6" s="147" t="inlineStr">
-        <is>
-          <t>HOLD</t>
-        </is>
-      </c>
-      <c r="S6" s="148" t="n">
-        <v>0</v>
-      </c>
-      <c r="T6" s="1651" t="n">
-        <v>0</v>
-      </c>
-      <c r="U6" s="1652" t="n">
-        <v>-0.02</v>
-      </c>
-      <c r="V6" s="151" t="inlineStr">
-        <is>
-          <t>TRUEFALSEFALSE</t>
-        </is>
-      </c>
-      <c r="W6" s="152" t="inlineStr">
-        <is>
-          <t>FALSEFALSETRUE</t>
-        </is>
-      </c>
-      <c r="X6" s="1653" t="n">
-        <v>90.90000000000001</v>
-      </c>
-      <c r="Y6" s="1654" t="n">
-        <v>91.37</v>
-      </c>
-      <c r="Z6" s="1655" t="n">
-        <v>91.47</v>
-      </c>
-      <c r="AA6" s="1656" t="n">
-        <v>91.37</v>
+      <c r="N6" s="143">
+        <f>IF($V6="TRUETRUETRUE","(!BUY!)","HOLD")</f>
+        <v/>
+      </c>
+      <c r="O6" s="144">
+        <f>ROUNDDOWN($AC6,0)</f>
+        <v/>
+      </c>
+      <c r="P6" s="1649">
+        <f>$O6*$G6</f>
+        <v/>
+      </c>
+      <c r="Q6" s="1650">
+        <f>MAX($J6:$M6)-$G6+0.01</f>
+        <v/>
+      </c>
+      <c r="R6" s="147">
+        <f>IF($W6="TRUETRUETRUE","!SELL!","HOLD")</f>
+        <v/>
+      </c>
+      <c r="S6" s="148">
+        <f>ROUNDDOWN($AD6,0)</f>
+        <v/>
+      </c>
+      <c r="T6" s="1651">
+        <f>$S6*$G6</f>
+        <v/>
+      </c>
+      <c r="U6" s="1652">
+        <f>MIN(J6:M6)-G6-0.01</f>
+        <v/>
+      </c>
+      <c r="V6" s="151">
+        <f>IF($G6&lt;$H6,$G6&lt;$I6)&amp;IF($G6&gt;$J6,$G6&gt;$K6)&amp;IF($G6&gt;$L6,$G6&gt;$M6)</f>
+        <v/>
+      </c>
+      <c r="W6" s="152">
+        <f>IF($G6&gt;$H6,$G6&gt;$I6)&amp;IF($G6&lt;$J6,$G6&lt;$K6)&amp;IF($G6&lt;$L6,$G6&lt;$M6)</f>
+        <v/>
+      </c>
+      <c r="X6" s="1653">
+        <f>IF(MAXA(H6:M6)&gt;MINA(H6:I6),MAXA(J6:M6))+0.01</f>
+        <v/>
+      </c>
+      <c r="Y6" s="1654">
+        <f>IF(MINA($H6:$I6)&gt;MAXA($J6:$M6),MINA($H6:$I6),MINA($J6:$M6))-0.01</f>
+        <v/>
+      </c>
+      <c r="Z6" s="1655">
+        <f>MAX($H6,$I6)+0.01</f>
+        <v/>
+      </c>
+      <c r="AA6" s="1656">
+        <f>IF(MINA($H6:$I6)&gt;MAXA($J6:$M6),MINA($H6:$I6),MINA($J6:$M6))-0.01</f>
+        <v/>
       </c>
       <c r="AB6" s="157" t="inlineStr">
         <is>
           <t>JNK</t>
         </is>
       </c>
-      <c r="AC6" s="1657" t="n">
-        <v>0</v>
-      </c>
-      <c r="AD6" s="1657" t="n">
-        <v>0</v>
+      <c r="AC6" s="1657">
+        <f>IF(N6="(!BUY!)",$G$3/$G$6,0)</f>
+        <v/>
+      </c>
+      <c r="AD6" s="1657">
+        <f>IF(R6="!SELL!",$G$3/$G$6,0)</f>
+        <v/>
       </c>
       <c r="AE6" s="159" t="n"/>
       <c r="AF6" s="160" t="n"/>
@@ -11488,7 +11499,7 @@
       <c r="D7" s="137" t="n"/>
       <c r="E7" s="138" t="inlineStr">
         <is>
-          <t>06/19</t>
+          <t>05/31</t>
         </is>
       </c>
       <c r="F7" s="139" t="inlineStr">
@@ -11497,86 +11508,94 @@
         </is>
       </c>
       <c r="G7" s="1646" t="n">
-        <v>31.39</v>
+        <v>30.31</v>
       </c>
       <c r="H7" s="1647" t="n">
-        <v>33</v>
+        <v>33.2</v>
       </c>
       <c r="I7" s="1648" t="n">
-        <v>29.17</v>
+        <v>28.83</v>
       </c>
       <c r="J7" s="1647" t="n">
-        <v>31.38</v>
+        <v>30.94</v>
       </c>
       <c r="K7" s="1648" t="n">
-        <v>31.08</v>
+        <v>30.54</v>
       </c>
       <c r="L7" s="1647" t="n">
-        <v>31.42</v>
+        <v>30.85</v>
       </c>
       <c r="M7" s="1648" t="n">
-        <v>31.41</v>
-      </c>
-      <c r="N7" s="147" t="inlineStr">
-        <is>
-          <t>HOLD</t>
-        </is>
-      </c>
-      <c r="O7" s="169" t="n">
-        <v>0</v>
-      </c>
-      <c r="P7" s="1661" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q7" s="1662" t="n">
-        <v>0.64</v>
-      </c>
-      <c r="R7" s="147" t="inlineStr">
-        <is>
-          <t>HOLD</t>
-        </is>
-      </c>
-      <c r="S7" s="148" t="n">
-        <v>0</v>
-      </c>
-      <c r="T7" s="1651" t="n">
-        <v>0</v>
-      </c>
-      <c r="U7" s="1652" t="n">
-        <v>0.22</v>
-      </c>
-      <c r="V7" s="151" t="inlineStr">
-        <is>
-          <t>FALSEFALSEFALSE</t>
-        </is>
-      </c>
-      <c r="W7" s="152" t="inlineStr">
-        <is>
-          <t>FALSETRUETRUE</t>
-        </is>
-      </c>
-      <c r="X7" s="1655" t="n">
-        <v>30.95</v>
-      </c>
-      <c r="Y7" s="1656" t="n">
-        <v>30.53</v>
-      </c>
-      <c r="Z7" s="1655" t="n">
-        <v>33.21</v>
-      </c>
-      <c r="AA7" s="1656" t="n">
-        <v>30.53</v>
+        <v>30.92</v>
+      </c>
+      <c r="N7" s="147">
+        <f>IF($V7="TRUETRUETRUE","(!BUY!)","HOLD")</f>
+        <v/>
+      </c>
+      <c r="O7" s="169">
+        <f>ROUNDDOWN($AC7,0)</f>
+        <v/>
+      </c>
+      <c r="P7" s="1661">
+        <f>$O7*$G7</f>
+        <v/>
+      </c>
+      <c r="Q7" s="1662">
+        <f>MAX($J7:$M7)-$G7+0.01</f>
+        <v/>
+      </c>
+      <c r="R7" s="147">
+        <f>IF($W7="TRUETRUETRUE","!SELL!","HOLD")</f>
+        <v/>
+      </c>
+      <c r="S7" s="148">
+        <f>ROUNDDOWN($AD7,0)</f>
+        <v/>
+      </c>
+      <c r="T7" s="1651">
+        <f>$S7*$G7</f>
+        <v/>
+      </c>
+      <c r="U7" s="1652">
+        <f>MIN(J7:M7)-G7-0.01</f>
+        <v/>
+      </c>
+      <c r="V7" s="151">
+        <f>IF($G7&lt;$H7,$G7&lt;$I7)&amp;IF($G7&gt;$J7,$G7&gt;$K7)&amp;IF($G7&gt;$L7,$G7&gt;$M7)</f>
+        <v/>
+      </c>
+      <c r="W7" s="152">
+        <f>IF($G7&gt;$H7,$G7&gt;$I7)&amp;IF($G7&lt;$J7,$G7&lt;$K7)&amp;IF($G7&lt;$L7,$G7&lt;$M7)</f>
+        <v/>
+      </c>
+      <c r="X7" s="1655">
+        <f>IF(MAXA(H7:M7)&gt;MINA(H7:I7),MAXA(J7:M7))+0.01</f>
+        <v/>
+      </c>
+      <c r="Y7" s="1656">
+        <f>IF(MINA($H7:$I7)&gt;MAXA($J7:$M7),MINA($H7:$I7),MINA($J7:$M7))-0.01</f>
+        <v/>
+      </c>
+      <c r="Z7" s="1655">
+        <f>MAX(H7,I7)+0.01</f>
+        <v/>
+      </c>
+      <c r="AA7" s="1656">
+        <f>IF(MINA($H$7:$I$7)&gt;MAXA($J$7:$M$7),MINA($H$7:$I$7),MINA($J$7:$M7))-0.01</f>
+        <v/>
       </c>
       <c r="AB7" s="157" t="inlineStr">
         <is>
           <t>GDX</t>
         </is>
       </c>
-      <c r="AC7" s="1657" t="n">
-        <v>0</v>
-      </c>
-      <c r="AD7" s="1663" t="n">
-        <v>0</v>
+      <c r="AC7" s="1657">
+        <f>IF(N7="(!BUY!)",$G$3/G7,0)</f>
+        <v/>
+      </c>
+      <c r="AD7" s="1663">
+        <f>IF(R7="!SELL!",$G$3/G7,0)</f>
+        <v/>
       </c>
       <c r="AE7" s="159" t="n"/>
       <c r="AF7" s="160" t="n"/>
@@ -11608,7 +11627,7 @@
       <c r="D8" s="137" t="n"/>
       <c r="E8" s="138" t="inlineStr">
         <is>
-          <t>06/19</t>
+          <t>05/31</t>
         </is>
       </c>
       <c r="F8" s="139" t="inlineStr">
@@ -11617,86 +11636,94 @@
         </is>
       </c>
       <c r="G8" s="1646" t="n">
-        <v>277.3</v>
+        <v>253.25</v>
       </c>
       <c r="H8" s="1647" t="n">
-        <v>254.69</v>
+        <v>248.76</v>
       </c>
       <c r="I8" s="1648" t="n">
-        <v>244.79</v>
+        <v>245.06</v>
       </c>
       <c r="J8" s="1647" t="n">
-        <v>278.2</v>
+        <v>252.73</v>
       </c>
       <c r="K8" s="1648" t="n">
-        <v>276.99</v>
+        <v>253.62</v>
       </c>
       <c r="L8" s="1647" t="n">
-        <v>278.01</v>
+        <v>251.96</v>
       </c>
       <c r="M8" s="1648" t="n">
-        <v>277.23</v>
-      </c>
-      <c r="N8" s="147" t="inlineStr">
-        <is>
-          <t>HOLD</t>
-        </is>
-      </c>
-      <c r="O8" s="169" t="n">
-        <v>0</v>
-      </c>
-      <c r="P8" s="1661" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q8" s="1662" t="n">
-        <v>1.54</v>
-      </c>
-      <c r="R8" s="179" t="inlineStr">
-        <is>
-          <t>HOLD</t>
-        </is>
-      </c>
-      <c r="S8" s="180" t="n">
-        <v>0</v>
-      </c>
-      <c r="T8" s="1667" t="n">
-        <v>0</v>
-      </c>
-      <c r="U8" s="1668" t="n">
-        <v>-1.3</v>
-      </c>
-      <c r="V8" s="151" t="inlineStr">
-        <is>
-          <t>FALSEFALSEFALSE</t>
-        </is>
-      </c>
-      <c r="W8" s="152" t="inlineStr">
-        <is>
-          <t>TRUEFALSEFALSE</t>
-        </is>
-      </c>
-      <c r="X8" s="1669" t="n">
-        <v>254.79</v>
-      </c>
-      <c r="Y8" s="1670" t="n">
-        <v>251.95</v>
-      </c>
-      <c r="Z8" s="1671" t="n">
-        <v>248.77</v>
-      </c>
-      <c r="AA8" s="1672" t="n">
-        <v>251.95</v>
+        <v>254.78</v>
+      </c>
+      <c r="N8" s="147">
+        <f>IF($V8="TRUETRUETRUE","(!BUY!)","HOLD")</f>
+        <v/>
+      </c>
+      <c r="O8" s="169">
+        <f>ROUNDDOWN($AC8,0)</f>
+        <v/>
+      </c>
+      <c r="P8" s="1661">
+        <f>$O8*$G8</f>
+        <v/>
+      </c>
+      <c r="Q8" s="1662">
+        <f>MAX(J8:M8)-G8+0.01</f>
+        <v/>
+      </c>
+      <c r="R8" s="179">
+        <f>IF(W8="TRUETRUETRUE","!SELL!","HOLD")</f>
+        <v/>
+      </c>
+      <c r="S8" s="180">
+        <f>ROUNDDOWN(AD8,0)</f>
+        <v/>
+      </c>
+      <c r="T8" s="1667">
+        <f>S8*G8</f>
+        <v/>
+      </c>
+      <c r="U8" s="1668">
+        <f>MIN(J8:M8)-G8-0.01</f>
+        <v/>
+      </c>
+      <c r="V8" s="151">
+        <f>IF($G8&lt;$H8,$G8&lt;$I8)&amp;IF($G8&gt;$J8,$G8&gt;$K8)&amp;IF($G8&gt;$L8,$G8&gt;$M8)</f>
+        <v/>
+      </c>
+      <c r="W8" s="152">
+        <f>IF($G8&gt;$H8,$G8&gt;$I8)&amp;IF($G8&lt;$J8,$G8&lt;$K8)&amp;IF($G8&lt;$L8,$G8&lt;$M8)</f>
+        <v/>
+      </c>
+      <c r="X8" s="1669">
+        <f>IF(MAXA(H8:M8)&gt;MINA(H8:I8),MAXA(J8:M8))+0.01</f>
+        <v/>
+      </c>
+      <c r="Y8" s="1670">
+        <f>IF(MINA($H8:$I8)&gt;MAXA($J8:$M8),MINA($H8:$I8),MINA($J8:$M8))-0.01</f>
+        <v/>
+      </c>
+      <c r="Z8" s="1671">
+        <f>MAX(H8,I8)+0.01</f>
+        <v/>
+      </c>
+      <c r="AA8" s="1672">
+        <f>IF(MINA($H$8:$I$8)&gt;MAXA($J$8:$M$8),MINA($H$8:$I$8),MINA($J$8:$M$8))-0.01</f>
+        <v/>
       </c>
       <c r="AB8" s="157" t="inlineStr">
         <is>
           <t>VCR</t>
         </is>
       </c>
-      <c r="AC8" s="1657" t="n">
-        <v>0</v>
-      </c>
-      <c r="AD8" s="1657" t="n">
-        <v>0</v>
+      <c r="AC8" s="1657">
+        <f>IF(N8="(!BUY!)",$G$3/G8,0)</f>
+        <v/>
+      </c>
+      <c r="AD8" s="1657">
+        <f>IF(R8="!SELL!",$G$3/G8,0)</f>
+        <v/>
       </c>
       <c r="AE8" s="159" t="n"/>
       <c r="AF8" s="160" t="n"/>
@@ -11727,7 +11754,7 @@
       <c r="D9" s="137" t="n"/>
       <c r="E9" s="138" t="inlineStr">
         <is>
-          <t>06/19</t>
+          <t>05/31</t>
         </is>
       </c>
       <c r="F9" s="139" t="inlineStr">
@@ -11736,86 +11763,94 @@
         </is>
       </c>
       <c r="G9" s="1646" t="n">
-        <v>195.57</v>
+        <v>189.6</v>
       </c>
       <c r="H9" s="1647" t="n">
-        <v>195.61</v>
+        <v>195.25</v>
       </c>
       <c r="I9" s="1648" t="n">
-        <v>190.02</v>
+        <v>190.21</v>
       </c>
       <c r="J9" s="1647" t="n">
-        <v>195.91</v>
+        <v>189.84</v>
       </c>
       <c r="K9" s="1648" t="n">
-        <v>195.03</v>
+        <v>189.94</v>
       </c>
       <c r="L9" s="1647" t="n">
-        <v>195.69</v>
+        <v>190.12</v>
       </c>
       <c r="M9" s="1648" t="n">
-        <v>195.94</v>
-      </c>
-      <c r="N9" s="143" t="inlineStr">
-        <is>
-          <t>HOLD</t>
-        </is>
-      </c>
-      <c r="O9" s="144" t="n">
-        <v>0</v>
-      </c>
-      <c r="P9" s="1649" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q9" s="1650" t="n">
-        <v>0.53</v>
-      </c>
-      <c r="R9" s="147" t="inlineStr">
-        <is>
-          <t>HOLD</t>
-        </is>
-      </c>
-      <c r="S9" s="148" t="n">
-        <v>0</v>
-      </c>
-      <c r="T9" s="1651" t="n">
-        <v>0</v>
-      </c>
-      <c r="U9" s="1652" t="n">
-        <v>-2.08166817117217e-19</v>
-      </c>
-      <c r="V9" s="151" t="inlineStr">
-        <is>
-          <t>TRUEFALSEFALSE</t>
-        </is>
-      </c>
-      <c r="W9" s="152" t="inlineStr">
-        <is>
-          <t>FALSETRUETRUE</t>
-        </is>
-      </c>
-      <c r="X9" s="1674" t="n">
-        <v>190.13</v>
-      </c>
-      <c r="Y9" s="1675" t="n">
-        <v>190.2</v>
-      </c>
-      <c r="Z9" s="1669" t="n">
-        <v>195.26</v>
-      </c>
-      <c r="AA9" s="1670" t="n">
-        <v>190.2</v>
+        <v>189.61</v>
+      </c>
+      <c r="N9" s="143">
+        <f>IF($V9="TRUETRUETRUE","(!BUY!)","HOLD")</f>
+        <v/>
+      </c>
+      <c r="O9" s="144">
+        <f>ROUNDDOWN($AC9,0)</f>
+        <v/>
+      </c>
+      <c r="P9" s="1649">
+        <f>$O9*$G9</f>
+        <v/>
+      </c>
+      <c r="Q9" s="1650">
+        <f>MAX(J9:M9)-G9+0.01</f>
+        <v/>
+      </c>
+      <c r="R9" s="147">
+        <f>IF(W9="TRUETRUETRUE","!SELL!","HOLD")</f>
+        <v/>
+      </c>
+      <c r="S9" s="148">
+        <f>ROUNDDOWN(AD9,0)</f>
+        <v/>
+      </c>
+      <c r="T9" s="1651">
+        <f>S9*G9</f>
+        <v/>
+      </c>
+      <c r="U9" s="1652">
+        <f>MIN(J9:M9)-G9-0.01</f>
+        <v/>
+      </c>
+      <c r="V9" s="151">
+        <f>IF($G9&lt;$H9,$G9&lt;$I9)&amp;IF($G9&gt;$J9,$G9&gt;$K9)&amp;IF($G9&gt;$L9,$G9&gt;$M9)</f>
+        <v/>
+      </c>
+      <c r="W9" s="152">
+        <f>IF($G9&gt;$H9,$G9&gt;$I9)&amp;IF($G9&lt;$J9,$G9&lt;$K9)&amp;IF($G9&lt;$L9,$G9&lt;$M9)</f>
+        <v/>
+      </c>
+      <c r="X9" s="1674">
+        <f>IF(MAXA(H9:M9)&gt;MINA(H9:I9),MAXA(J9:M9))+0.01</f>
+        <v/>
+      </c>
+      <c r="Y9" s="1675">
+        <f>IF(MINA($H9:$I9)&gt;MAXA($J9:$M9),MINA($H9:$I9),MINA($J9:$M9))-0.01</f>
+        <v/>
+      </c>
+      <c r="Z9" s="1669">
+        <f>MAX(H9,I9)+0.01</f>
+        <v/>
+      </c>
+      <c r="AA9" s="1670">
+        <f>IF(MINA($H$9:$I$9)&gt;MAXA($J$9:$M$9),MINA($H$9:$I$9),MINA($J$9:$M$9))-0.01</f>
+        <v/>
       </c>
       <c r="AB9" s="157" t="inlineStr">
         <is>
           <t>VDC</t>
         </is>
       </c>
-      <c r="AC9" s="1657" t="n">
-        <v>0</v>
-      </c>
-      <c r="AD9" s="1657" t="n">
-        <v>0</v>
+      <c r="AC9" s="1657">
+        <f>IF(N9="(!BUY!)",$G$3/G9,0)</f>
+        <v/>
+      </c>
+      <c r="AD9" s="1657">
+        <f>IF(R9="!SELL!",$G$3/G9,0)</f>
+        <v/>
       </c>
       <c r="AE9" s="159" t="n"/>
       <c r="AF9" s="160" t="n"/>
@@ -11895,7 +11930,7 @@
       <c r="D11" s="137" t="n"/>
       <c r="E11" s="138" t="inlineStr">
         <is>
-          <t>06/19</t>
+          <t>05/31</t>
         </is>
       </c>
       <c r="F11" s="139" t="inlineStr">
@@ -11904,86 +11939,94 @@
         </is>
       </c>
       <c r="G11" s="1646" t="n">
-        <v>161.25</v>
+        <v>153.25</v>
       </c>
       <c r="H11" s="1647" t="n">
-        <v>156.08</v>
+        <v>154.47</v>
       </c>
       <c r="I11" s="1648" t="n">
-        <v>151.69</v>
+        <v>151.51</v>
       </c>
       <c r="J11" s="1647" t="n">
-        <v>161.66</v>
+        <v>153.28</v>
       </c>
       <c r="K11" s="1648" t="n">
-        <v>160.95</v>
+        <v>153.8</v>
       </c>
       <c r="L11" s="1647" t="n">
-        <v>161.3</v>
+        <v>153.45</v>
       </c>
       <c r="M11" s="1648" t="n">
-        <v>161.63</v>
-      </c>
-      <c r="N11" s="147" t="inlineStr">
-        <is>
-          <t>HOLD</t>
-        </is>
-      </c>
-      <c r="O11" s="169" t="n">
-        <v>0</v>
-      </c>
-      <c r="P11" s="1661" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q11" s="1662" t="n">
-        <v>0.5600000000000001</v>
-      </c>
-      <c r="R11" s="147" t="inlineStr">
-        <is>
-          <t>HOLD</t>
-        </is>
-      </c>
-      <c r="S11" s="148" t="n">
-        <v>0</v>
-      </c>
-      <c r="T11" s="1651" t="n">
-        <v>0</v>
-      </c>
-      <c r="U11" s="1652" t="n">
-        <v>0.02</v>
-      </c>
-      <c r="V11" s="151" t="inlineStr">
-        <is>
-          <t>FALSEFALSEFALSE</t>
-        </is>
-      </c>
-      <c r="W11" s="152" t="inlineStr">
-        <is>
-          <t>FALSETRUETRUE</t>
-        </is>
-      </c>
-      <c r="X11" s="1669" t="n">
-        <v>153.81</v>
-      </c>
-      <c r="Y11" s="1670" t="n">
-        <v>153.27</v>
-      </c>
-      <c r="Z11" s="1669" t="n">
-        <v>154.48</v>
-      </c>
-      <c r="AA11" s="1670" t="n">
-        <v>153.27</v>
+        <v>153.33</v>
+      </c>
+      <c r="N11" s="147">
+        <f>IF($V11="TRUETRUETRUE","(!BUY!)","HOLD")</f>
+        <v/>
+      </c>
+      <c r="O11" s="169">
+        <f>ROUNDDOWN($AC11,0)</f>
+        <v/>
+      </c>
+      <c r="P11" s="1661">
+        <f>$O11*$G11</f>
+        <v/>
+      </c>
+      <c r="Q11" s="1662">
+        <f>MAX(J11:M11)-G11+0.01</f>
+        <v/>
+      </c>
+      <c r="R11" s="147">
+        <f>IF(W11="TRUETRUETRUE","!SELL!","HOLD")</f>
+        <v/>
+      </c>
+      <c r="S11" s="148">
+        <f>ROUNDDOWN(AD11,0)</f>
+        <v/>
+      </c>
+      <c r="T11" s="1651">
+        <f>S11*G11</f>
+        <v/>
+      </c>
+      <c r="U11" s="1652">
+        <f>MIN(J11:M11)-G11-0.01</f>
+        <v/>
+      </c>
+      <c r="V11" s="151">
+        <f>IF($G11&lt;$H11,$G11&lt;$I11)&amp;IF($G11&gt;$J11,$G11&gt;$K11)&amp;IF($G11&gt;$L11,$G11&gt;$M11)</f>
+        <v/>
+      </c>
+      <c r="W11" s="152">
+        <f>IF($G11&gt;$H11,$G11&gt;$I11)&amp;IF($G11&lt;$J11,$G11&lt;$K11)&amp;IF($G11&lt;$L11,$G11&lt;$M11)</f>
+        <v/>
+      </c>
+      <c r="X11" s="1669">
+        <f>IF(MAXA(H11:M11)&gt;MINA(H11:I11),MAXA(J11:M11))+0.01</f>
+        <v/>
+      </c>
+      <c r="Y11" s="1670">
+        <f>IF(MINA($H11:$I11)&gt;MAXA($J11:$M11),MINA($H11:$I11),MINA($J11:$M11))-0.01</f>
+        <v/>
+      </c>
+      <c r="Z11" s="1669">
+        <f>MAX(H11,I11)+0.01</f>
+        <v/>
+      </c>
+      <c r="AA11" s="1670">
+        <f>IF(MINA($H$11:$I$11)&gt;MAXA($J$11:$M$11),MINA($H$11:$I$11),MINA($J$11:$M$11))-0.01</f>
+        <v/>
       </c>
       <c r="AB11" s="157" t="inlineStr">
         <is>
           <t>VIG</t>
         </is>
       </c>
-      <c r="AC11" s="1657" t="n">
-        <v>0</v>
-      </c>
-      <c r="AD11" s="1657" t="n">
-        <v>0</v>
+      <c r="AC11" s="1657">
+        <f>IF(N11="(!BUY!)",$G$3/G11,0)</f>
+        <v/>
+      </c>
+      <c r="AD11" s="1657">
+        <f>IF(R11="!SELL!",$G$3/G11,0)</f>
+        <v/>
       </c>
       <c r="AE11" s="159" t="n"/>
       <c r="AF11" s="160" t="n"/>
@@ -12016,7 +12059,7 @@
       <c r="D12" s="137" t="n"/>
       <c r="E12" s="138" t="inlineStr">
         <is>
-          <t>06/19</t>
+          <t>05/31</t>
         </is>
       </c>
       <c r="F12" s="139" t="inlineStr">
@@ -12025,86 +12068,94 @@
         </is>
       </c>
       <c r="G12" s="1646" t="n">
-        <v>112.24</v>
+        <v>105.87</v>
       </c>
       <c r="H12" s="1647" t="n">
-        <v>112.58</v>
+        <v>112.95</v>
       </c>
       <c r="I12" s="1648" t="n">
-        <v>116.99</v>
+        <v>117.12</v>
       </c>
       <c r="J12" s="1647" t="n">
-        <v>112.58</v>
+        <v>105.97</v>
       </c>
       <c r="K12" s="1648" t="n">
-        <v>112.16</v>
+        <v>107.13</v>
       </c>
       <c r="L12" s="1647" t="n">
-        <v>112.21</v>
+        <v>105.88</v>
       </c>
       <c r="M12" s="1648" t="n">
-        <v>112.62</v>
-      </c>
-      <c r="N12" s="143" t="inlineStr">
-        <is>
-          <t>HOLD</t>
-        </is>
-      </c>
-      <c r="O12" s="144" t="n">
-        <v>0</v>
-      </c>
-      <c r="P12" s="1649" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q12" s="1685" t="n">
-        <v>1.27</v>
-      </c>
-      <c r="R12" s="147" t="inlineStr">
-        <is>
-          <t>HOLD</t>
-        </is>
-      </c>
-      <c r="S12" s="148" t="n">
-        <v>0</v>
-      </c>
-      <c r="T12" s="1651" t="n">
-        <v>0</v>
-      </c>
-      <c r="U12" s="1652" t="n">
-        <v>-2.08166817117217e-19</v>
-      </c>
-      <c r="V12" s="151" t="inlineStr">
-        <is>
-          <t>TRUEFALSEFALSE</t>
-        </is>
-      </c>
-      <c r="W12" s="152" t="inlineStr">
-        <is>
-          <t>FALSETRUETRUE</t>
-        </is>
-      </c>
-      <c r="X12" s="1674" t="n">
-        <v>107.14</v>
-      </c>
-      <c r="Y12" s="1675" t="n">
-        <v>112.94</v>
-      </c>
-      <c r="Z12" s="1669" t="n">
-        <v>117.13</v>
-      </c>
-      <c r="AA12" s="1670" t="n">
-        <v>112.94</v>
+        <v>105.96</v>
+      </c>
+      <c r="N12" s="143">
+        <f>IF($V12="TRUETRUETRUE","(!BUY!)","HOLD")</f>
+        <v/>
+      </c>
+      <c r="O12" s="144">
+        <f>ROUNDDOWN($AC12,0)</f>
+        <v/>
+      </c>
+      <c r="P12" s="1649">
+        <f>$O12*$G12</f>
+        <v/>
+      </c>
+      <c r="Q12" s="1685">
+        <f>MAX(J12:M12)-G12+0.01</f>
+        <v/>
+      </c>
+      <c r="R12" s="147">
+        <f>IF(W12="TRUETRUETRUE","!SELL!","HOLD")</f>
+        <v/>
+      </c>
+      <c r="S12" s="148">
+        <f>ROUNDDOWN(AD12,0)</f>
+        <v/>
+      </c>
+      <c r="T12" s="1651">
+        <f>S12*G12</f>
+        <v/>
+      </c>
+      <c r="U12" s="1652">
+        <f>MIN(J12:M12)-G12-0.01</f>
+        <v/>
+      </c>
+      <c r="V12" s="151">
+        <f>IF($G12&lt;$H12,$G12&lt;$I12)&amp;IF($G12&gt;$J12,$G12&gt;$K12)&amp;IF($G12&gt;$L12,$G12&gt;$M12)</f>
+        <v/>
+      </c>
+      <c r="W12" s="152">
+        <f>IF($G12&gt;$H12,$G12&gt;$I12)&amp;IF($G12&lt;$J12,$G12&lt;$K12)&amp;IF($G12&lt;$L12,$G12&lt;$M12)</f>
+        <v/>
+      </c>
+      <c r="X12" s="1674">
+        <f>IF(MAXA(H12:M12)&gt;MINA(H12:I12),MAXA(J12:M12))+0.01</f>
+        <v/>
+      </c>
+      <c r="Y12" s="1675">
+        <f>IF(MINA($H12:$I12)&gt;MAXA($J12:$M12),MINA($H12:$I12),MINA($J12:$M12))-0.01</f>
+        <v/>
+      </c>
+      <c r="Z12" s="1669">
+        <f>MAX(H12,I12)+0.01</f>
+        <v/>
+      </c>
+      <c r="AA12" s="1670">
+        <f>IF(MINA($H$12:$I$12)&gt;MAXA($J$12:$M$12),MINA($H$12:$I$12),MINA($J$12:$M$12))-0.01</f>
+        <v/>
       </c>
       <c r="AB12" s="157" t="inlineStr">
         <is>
           <t>VDE</t>
         </is>
       </c>
-      <c r="AC12" s="1657" t="n">
-        <v>0</v>
-      </c>
-      <c r="AD12" s="1657" t="n">
-        <v>0</v>
+      <c r="AC12" s="1657">
+        <f>IF(N12="(!BUY!)",$G$3/G12,0)</f>
+        <v/>
+      </c>
+      <c r="AD12" s="1657">
+        <f>IF(R12="!SELL!",$G$3/G12,0)</f>
+        <v/>
       </c>
       <c r="AE12" s="159" t="n"/>
       <c r="AF12" s="160" t="n"/>
@@ -12140,7 +12191,7 @@
       <c r="D13" s="137" t="n"/>
       <c r="E13" s="138" t="inlineStr">
         <is>
-          <t>06/19</t>
+          <t>05/31</t>
         </is>
       </c>
       <c r="F13" s="139" t="inlineStr">
@@ -12149,86 +12200,94 @@
         </is>
       </c>
       <c r="G13" s="1646" t="n">
-        <v>81.2</v>
+        <v>76.44</v>
       </c>
       <c r="H13" s="1647" t="n">
-        <v>78.28</v>
+        <v>77.48</v>
       </c>
       <c r="I13" s="1648" t="n">
-        <v>81.78</v>
+        <v>82.09999999999999</v>
       </c>
       <c r="J13" s="1647" t="n">
-        <v>81.39</v>
+        <v>76.36</v>
       </c>
       <c r="K13" s="1648" t="n">
-        <v>81.12</v>
+        <v>76.90000000000001</v>
       </c>
       <c r="L13" s="1647" t="n">
-        <v>81.23</v>
+        <v>76.53</v>
       </c>
       <c r="M13" s="1648" t="n">
-        <v>81.36</v>
-      </c>
-      <c r="N13" s="143" t="inlineStr">
-        <is>
-          <t>HOLD</t>
-        </is>
-      </c>
-      <c r="O13" s="144" t="n">
-        <v>0</v>
-      </c>
-      <c r="P13" s="1649" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q13" s="1650" t="n">
-        <v>0.47</v>
-      </c>
-      <c r="R13" s="147" t="inlineStr">
-        <is>
-          <t>HOLD</t>
-        </is>
-      </c>
-      <c r="S13" s="148" t="n">
-        <v>0</v>
-      </c>
-      <c r="T13" s="1651" t="n">
-        <v>0</v>
-      </c>
-      <c r="U13" s="1652" t="n">
-        <v>-0.1</v>
-      </c>
-      <c r="V13" s="151" t="inlineStr">
-        <is>
-          <t>TRUEFALSEFALSE</t>
-        </is>
-      </c>
-      <c r="W13" s="152" t="inlineStr">
-        <is>
-          <t>FALSEFALSEFALSE</t>
-        </is>
-      </c>
-      <c r="X13" s="1653" t="n">
-        <v>76.91</v>
-      </c>
-      <c r="Y13" s="1654" t="n">
-        <v>77.47</v>
-      </c>
-      <c r="Z13" s="1655" t="n">
-        <v>82.11</v>
-      </c>
-      <c r="AA13" s="1656" t="n">
-        <v>77.47</v>
+        <v>76.34999999999999</v>
+      </c>
+      <c r="N13" s="143">
+        <f>IF($V13="TRUETRUETRUE","(!BUY!)","HOLD")</f>
+        <v/>
+      </c>
+      <c r="O13" s="144">
+        <f>ROUNDDOWN($AC13,0)</f>
+        <v/>
+      </c>
+      <c r="P13" s="1649">
+        <f>$O13*$G13</f>
+        <v/>
+      </c>
+      <c r="Q13" s="1650">
+        <f>MAX(J13:M13)-G13+0.01</f>
+        <v/>
+      </c>
+      <c r="R13" s="147">
+        <f>IF(W13="TRUETRUETRUE","!SELL!","HOLD")</f>
+        <v/>
+      </c>
+      <c r="S13" s="148">
+        <f>ROUNDDOWN(AD13,0)</f>
+        <v/>
+      </c>
+      <c r="T13" s="1651">
+        <f>S13*G13</f>
+        <v/>
+      </c>
+      <c r="U13" s="1652">
+        <f>MIN(J13:M13)-G13-0.01</f>
+        <v/>
+      </c>
+      <c r="V13" s="151">
+        <f>IF($G13&lt;$H13,$G13&lt;$I13)&amp;IF($G13&gt;$J13,$G13&gt;$K13)&amp;IF($G13&gt;$L13,$G13&gt;$M13)</f>
+        <v/>
+      </c>
+      <c r="W13" s="152">
+        <f>IF($G13&gt;$H13,$G13&gt;$I13)&amp;IF($G13&lt;$J13,$G13&lt;$K13)&amp;IF($G13&lt;$L13,$G13&lt;$M13)</f>
+        <v/>
+      </c>
+      <c r="X13" s="1653">
+        <f>IF(MAXA(H13:M13)&gt;MINA(H13:I13),MAXA(J13:M13))+0.01</f>
+        <v/>
+      </c>
+      <c r="Y13" s="1654">
+        <f>IF(MINA($H13:$I13)&gt;MAXA($J13:$M13),MINA($H13:$I13),MINA($J13:$M13))-0.01</f>
+        <v/>
+      </c>
+      <c r="Z13" s="1655">
+        <f>MAX(H13,I13)+0.01</f>
+        <v/>
+      </c>
+      <c r="AA13" s="1656">
+        <f>IF(MINA($H$13:$I$13)&gt;MAXA($J$13:$M$13),MINA($H$13:$I$13),MINA($J$13:$M$13))-0.01</f>
+        <v/>
       </c>
       <c r="AB13" s="157" t="inlineStr">
         <is>
           <t>VFH</t>
         </is>
       </c>
-      <c r="AC13" s="1657" t="n">
-        <v>0</v>
-      </c>
-      <c r="AD13" s="1657" t="n">
-        <v>0</v>
+      <c r="AC13" s="1657">
+        <f>IF(N13="(!BUY!)",$G$3/G13,0)</f>
+        <v/>
+      </c>
+      <c r="AD13" s="1657">
+        <f>IF(R13="!SELL!",$G$3/G13,0)</f>
+        <v/>
       </c>
       <c r="AE13" s="159" t="n"/>
       <c r="AF13" s="160" t="n"/>
@@ -12264,7 +12323,7 @@
       <c r="D14" s="137" t="n"/>
       <c r="E14" s="138" t="inlineStr">
         <is>
-          <t>06/19</t>
+          <t>05/31</t>
         </is>
       </c>
       <c r="F14" s="139" t="inlineStr">
@@ -12273,86 +12332,94 @@
         </is>
       </c>
       <c r="G14" s="1646" t="n">
-        <v>41.94</v>
+        <v>39.05</v>
       </c>
       <c r="H14" s="1647" t="n">
-        <v>40.26</v>
+        <v>40.04</v>
       </c>
       <c r="I14" s="1648" t="n">
-        <v>39.64</v>
+        <v>39.69</v>
       </c>
       <c r="J14" s="1647" t="n">
-        <v>41.97</v>
+        <v>38.93</v>
       </c>
       <c r="K14" s="1648" t="n">
-        <v>41.91</v>
+        <v>39.29</v>
       </c>
       <c r="L14" s="1647" t="n">
-        <v>41.95</v>
+        <v>39.02</v>
       </c>
       <c r="M14" s="1648" t="n">
-        <v>41.98</v>
-      </c>
-      <c r="N14" s="143" t="inlineStr">
-        <is>
-          <t>HOLD</t>
-        </is>
-      </c>
-      <c r="O14" s="144" t="n">
-        <v>0</v>
-      </c>
-      <c r="P14" s="1649" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q14" s="1650" t="n">
-        <v>0.25</v>
-      </c>
-      <c r="R14" s="147" t="inlineStr">
-        <is>
-          <t>HOLD</t>
-        </is>
-      </c>
-      <c r="S14" s="148" t="n">
-        <v>0</v>
-      </c>
-      <c r="T14" s="1651" t="n">
-        <v>0</v>
-      </c>
-      <c r="U14" s="1652" t="n">
-        <v>-0.13</v>
-      </c>
-      <c r="V14" s="151" t="inlineStr">
-        <is>
-          <t>TRUEFALSETRUE</t>
-        </is>
-      </c>
-      <c r="W14" s="152" t="inlineStr">
-        <is>
-          <t>FALSEFALSEFALSE</t>
-        </is>
-      </c>
-      <c r="X14" s="1653" t="n">
-        <v>39.3</v>
-      </c>
-      <c r="Y14" s="1654" t="n">
-        <v>39.68</v>
-      </c>
-      <c r="Z14" s="1655" t="n">
-        <v>40.05</v>
-      </c>
-      <c r="AA14" s="1656" t="n">
-        <v>39.68</v>
+        <v>38.96</v>
+      </c>
+      <c r="N14" s="143">
+        <f>IF($V14="TRUETRUETRUE","(!BUY!)","HOLD")</f>
+        <v/>
+      </c>
+      <c r="O14" s="144">
+        <f>ROUNDDOWN($AC14,0)</f>
+        <v/>
+      </c>
+      <c r="P14" s="1649">
+        <f>$O14*$G14</f>
+        <v/>
+      </c>
+      <c r="Q14" s="1650">
+        <f>MAX(J14:M14)-G14+0.01</f>
+        <v/>
+      </c>
+      <c r="R14" s="147">
+        <f>IF(W14="TRUETRUETRUE","!SELL!","HOLD")</f>
+        <v/>
+      </c>
+      <c r="S14" s="148">
+        <f>ROUNDDOWN(AD14,0)</f>
+        <v/>
+      </c>
+      <c r="T14" s="1651">
+        <f>S14*G14</f>
+        <v/>
+      </c>
+      <c r="U14" s="1652">
+        <f>MIN(J14:M14)-G14-0.01</f>
+        <v/>
+      </c>
+      <c r="V14" s="151">
+        <f>IF($G14&lt;$H14,$G14&lt;$I14)&amp;IF($G14&gt;$J14,$G14&gt;$K14)&amp;IF($G14&gt;$L14,$G14&gt;$M14)</f>
+        <v/>
+      </c>
+      <c r="W14" s="152">
+        <f>IF($G14&gt;$H14,$G14&gt;$I14)&amp;IF($G14&lt;$J14,$G14&lt;$K14)&amp;IF($G14&lt;$L14,$G14&lt;$M14)</f>
+        <v/>
+      </c>
+      <c r="X14" s="1653">
+        <f>IF(MAXA(H14:M14)&gt;MINA(H14:I14),MAXA(J14:M14))+0.01</f>
+        <v/>
+      </c>
+      <c r="Y14" s="1654">
+        <f>IF(MINA($H$14:$I$14)&gt;MAXA($J$14:$M$14),MINA($H$14:$I$14),MINA($J$14:$M$14))-0.01</f>
+        <v/>
+      </c>
+      <c r="Z14" s="1655">
+        <f>MAX(H14,I14)+0.01</f>
+        <v/>
+      </c>
+      <c r="AA14" s="1656">
+        <f>IF(MINA($H$14:$I$14)&gt;MAXA($J$14:$M$14),MINA($H$14:$I$14),MINA($J$14:$M$14))-0.01</f>
+        <v/>
       </c>
       <c r="AB14" s="157" t="inlineStr">
         <is>
           <t>VWO</t>
         </is>
       </c>
-      <c r="AC14" s="1657" t="n">
-        <v>0</v>
-      </c>
-      <c r="AD14" s="1657" t="n">
-        <v>0</v>
+      <c r="AC14" s="1657">
+        <f>IF(N14="(!BUY!)",$G$3/G14,0)</f>
+        <v/>
+      </c>
+      <c r="AD14" s="1657">
+        <f>IF(R14="!SELL!",$G$3/G14,0)</f>
+        <v/>
       </c>
       <c r="AE14" s="159" t="n"/>
       <c r="AF14" s="160" t="n"/>
@@ -12449,7 +12516,7 @@
       <c r="D16" s="137" t="n"/>
       <c r="E16" s="138" t="inlineStr">
         <is>
-          <t>06/19</t>
+          <t>05/31</t>
         </is>
       </c>
       <c r="F16" s="139" t="inlineStr">
@@ -12458,86 +12525,94 @@
         </is>
       </c>
       <c r="G16" s="1646" t="n">
-        <v>244.53</v>
+        <v>235.86</v>
       </c>
       <c r="H16" s="1647" t="n">
-        <v>243.28</v>
+        <v>242.06</v>
       </c>
       <c r="I16" s="1648" t="n">
-        <v>240.97</v>
+        <v>241.03</v>
       </c>
       <c r="J16" s="1647" t="n">
-        <v>244.86</v>
+        <v>235.01</v>
       </c>
       <c r="K16" s="1648" t="n">
-        <v>243.69</v>
+        <v>234.77</v>
       </c>
       <c r="L16" s="1647" t="n">
-        <v>244.66</v>
+        <v>235.82</v>
       </c>
       <c r="M16" s="1648" t="n">
-        <v>245.06</v>
-      </c>
-      <c r="N16" s="227" t="inlineStr">
-        <is>
-          <t>(!BUY!)</t>
-        </is>
-      </c>
-      <c r="O16" s="228" t="n">
-        <v>4</v>
-      </c>
-      <c r="P16" s="1688" t="n">
-        <v>943.4400000000001</v>
-      </c>
-      <c r="Q16" s="1689" t="n">
-        <v>-0.03</v>
-      </c>
-      <c r="R16" s="147" t="inlineStr">
-        <is>
-          <t>HOLD</t>
-        </is>
-      </c>
-      <c r="S16" s="148" t="n">
-        <v>0</v>
-      </c>
-      <c r="T16" s="1651" t="n">
-        <v>0</v>
-      </c>
-      <c r="U16" s="1652" t="n">
-        <v>-1.17</v>
-      </c>
-      <c r="V16" s="151" t="inlineStr">
-        <is>
-          <t>TRUETRUETRUE</t>
-        </is>
-      </c>
-      <c r="W16" s="152" t="inlineStr">
-        <is>
-          <t>FALSEFALSEFALSE</t>
-        </is>
-      </c>
-      <c r="X16" s="1690" t="n">
-        <v>235.83</v>
-      </c>
-      <c r="Y16" s="1691" t="n">
-        <v>241.02</v>
-      </c>
-      <c r="Z16" s="1669" t="n">
-        <v>242.07</v>
-      </c>
-      <c r="AA16" s="1670" t="n">
-        <v>241.02</v>
+        <v>234.7</v>
+      </c>
+      <c r="N16" s="227">
+        <f>IF($V16="TRUETRUETRUE","(!BUY!)","HOLD")</f>
+        <v/>
+      </c>
+      <c r="O16" s="228">
+        <f>ROUNDDOWN($AC16,0)</f>
+        <v/>
+      </c>
+      <c r="P16" s="1688">
+        <f>$O16*$G16</f>
+        <v/>
+      </c>
+      <c r="Q16" s="1689">
+        <f>MAX(J16:M16)-G16+0.01</f>
+        <v/>
+      </c>
+      <c r="R16" s="147">
+        <f>IF(W16="TRUETRUETRUE","!SELL!","HOLD")</f>
+        <v/>
+      </c>
+      <c r="S16" s="148">
+        <f>ROUNDDOWN(AD16,0)</f>
+        <v/>
+      </c>
+      <c r="T16" s="1651">
+        <f>S16*G16</f>
+        <v/>
+      </c>
+      <c r="U16" s="1652">
+        <f>MIN(J16:M16)-G16-0.01</f>
+        <v/>
+      </c>
+      <c r="V16" s="151">
+        <f>IF($G16&lt;$H16,$G16&lt;$I16)&amp;IF($G16&gt;$J16,$G16&gt;$K16)&amp;IF($G16&gt;$L16,$G16&gt;$M16)</f>
+        <v/>
+      </c>
+      <c r="W16" s="152">
+        <f>IF($G16&gt;$H16,$G16&gt;$I16)&amp;IF($G16&lt;$J16,$G16&lt;$K16)&amp;IF($G16&lt;$L16,$G16&lt;$M16)</f>
+        <v/>
+      </c>
+      <c r="X16" s="1690">
+        <f>IF(MAXA(H16:M16)&gt;MINA(H16:I16),MAXA(J16:M16))+0.01</f>
+        <v/>
+      </c>
+      <c r="Y16" s="1691">
+        <f>IF(MINA($H16:$I16)&gt;MAXA($J16:$M16),MINA($H16:$I16),MINA($J16:$M16))-0.01</f>
+        <v/>
+      </c>
+      <c r="Z16" s="1669">
+        <f>MAX(H16,I16)+0.01</f>
+        <v/>
+      </c>
+      <c r="AA16" s="1670">
+        <f>IF(MINA($H$16:$I$16)&gt;MAXA($J$16:$M$16),MINA($H$16:$I$16),MINA($J$16:$M$16))-0.01</f>
+        <v/>
       </c>
       <c r="AB16" s="157" t="inlineStr">
         <is>
           <t>VHT</t>
         </is>
       </c>
-      <c r="AC16" s="1657" t="n">
-        <v>4.23980327312813</v>
-      </c>
-      <c r="AD16" s="1657" t="n">
-        <v>0</v>
+      <c r="AC16" s="1657">
+        <f>IF(N16="(!BUY!)",$G$3/G16,0)</f>
+        <v/>
+      </c>
+      <c r="AD16" s="1657">
+        <f>IF(R16="!SELL!",$G$3/G16,0)</f>
+        <v/>
       </c>
       <c r="AE16" s="159" t="n"/>
       <c r="AF16" s="160" t="n"/>
@@ -12572,7 +12647,7 @@
       <c r="D17" s="137" t="n"/>
       <c r="E17" s="138" t="inlineStr">
         <is>
-          <t>06/19</t>
+          <t>05/31</t>
         </is>
       </c>
       <c r="F17" s="139" t="inlineStr">
@@ -12581,86 +12656,94 @@
         </is>
       </c>
       <c r="G17" s="1646" t="n">
-        <v>201.18</v>
+        <v>184.11</v>
       </c>
       <c r="H17" s="1647" t="n">
-        <v>189.55</v>
+        <v>187.17</v>
       </c>
       <c r="I17" s="1648" t="n">
-        <v>184.14</v>
+        <v>183.51</v>
       </c>
       <c r="J17" s="1647" t="n">
-        <v>201.4</v>
+        <v>184.34</v>
       </c>
       <c r="K17" s="1648" t="n">
-        <v>200.34</v>
+        <v>186.05</v>
       </c>
       <c r="L17" s="1647" t="n">
-        <v>201.26</v>
+        <v>184.42</v>
       </c>
       <c r="M17" s="1648" t="n">
-        <v>201.11</v>
-      </c>
-      <c r="N17" s="147" t="inlineStr">
-        <is>
-          <t>HOLD</t>
-        </is>
-      </c>
-      <c r="O17" s="169" t="n">
-        <v>0</v>
-      </c>
-      <c r="P17" s="1661" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q17" s="1694" t="n">
-        <v>1.95</v>
-      </c>
-      <c r="R17" s="147" t="inlineStr">
-        <is>
-          <t>HOLD</t>
-        </is>
-      </c>
-      <c r="S17" s="148" t="n">
-        <v>0</v>
-      </c>
-      <c r="T17" s="1651" t="n">
-        <v>0</v>
-      </c>
-      <c r="U17" s="1652" t="n">
-        <v>0.22</v>
-      </c>
-      <c r="V17" s="151" t="inlineStr">
-        <is>
-          <t>FALSEFALSEFALSE</t>
-        </is>
-      </c>
-      <c r="W17" s="152" t="inlineStr">
-        <is>
-          <t>FALSETRUETRUE</t>
-        </is>
-      </c>
-      <c r="X17" s="1669" t="n">
-        <v>186.06</v>
-      </c>
-      <c r="Y17" s="1670" t="n">
-        <v>184.33</v>
-      </c>
-      <c r="Z17" s="1669" t="n">
-        <v>187.18</v>
-      </c>
-      <c r="AA17" s="1670" t="n">
-        <v>184.33</v>
+        <v>185.74</v>
+      </c>
+      <c r="N17" s="147">
+        <f>IF($V17="TRUETRUETRUE","(!BUY!)","HOLD")</f>
+        <v/>
+      </c>
+      <c r="O17" s="169">
+        <f>ROUNDDOWN($AC17,0)</f>
+        <v/>
+      </c>
+      <c r="P17" s="1661">
+        <f>$O17*$G17</f>
+        <v/>
+      </c>
+      <c r="Q17" s="1694">
+        <f>MAX(J17:M17)-G17+0.01</f>
+        <v/>
+      </c>
+      <c r="R17" s="147">
+        <f>IF(W17="TRUETRUETRUE","!SELL!","HOLD")</f>
+        <v/>
+      </c>
+      <c r="S17" s="148">
+        <f>ROUNDDOWN(AD17,0)</f>
+        <v/>
+      </c>
+      <c r="T17" s="1651">
+        <f>S17*G17</f>
+        <v/>
+      </c>
+      <c r="U17" s="1652">
+        <f>MIN(J17:M17)-G17-0.01</f>
+        <v/>
+      </c>
+      <c r="V17" s="151">
+        <f>IF($G17&lt;$H17,$G17&lt;$I17)&amp;IF($G17&gt;$J17,$G17&gt;$K17)&amp;IF($G17&gt;$L17,$G17&gt;$M17)</f>
+        <v/>
+      </c>
+      <c r="W17" s="152">
+        <f>IF($G17&gt;$H17,$G17&gt;$I17)&amp;IF($G17&lt;$J17,$G17&lt;$K17)&amp;IF($G17&lt;$L17,$G17&lt;$M17)</f>
+        <v/>
+      </c>
+      <c r="X17" s="1669">
+        <f>IF(MAXA(H17:M17)&gt;MINA(H17:I17),MAXA(J17:M17))+0.01</f>
+        <v/>
+      </c>
+      <c r="Y17" s="1670">
+        <f>IF(MINA($H17:$I17)&gt;MAXA($J17:$M17),MINA($H17:$I17),MINA($J17:$M17))-0.01</f>
+        <v/>
+      </c>
+      <c r="Z17" s="1669">
+        <f>MAX(H17,I17)+0.01</f>
+        <v/>
+      </c>
+      <c r="AA17" s="1670">
+        <f>IF(MINA($H$17:$I$17)&gt;MAXA($J$17:$M$17),MINA($H$17:$I$17),MINA($J$17:$M$17))-0.01</f>
+        <v/>
       </c>
       <c r="AB17" s="157" t="inlineStr">
         <is>
           <t>VIS</t>
         </is>
       </c>
-      <c r="AC17" s="1657" t="n">
-        <v>0</v>
-      </c>
-      <c r="AD17" s="1657" t="n">
-        <v>0</v>
+      <c r="AC17" s="1657">
+        <f>IF(N17="(!BUY!)",$G$3/G17,0)</f>
+        <v/>
+      </c>
+      <c r="AD17" s="1657">
+        <f>IF(R17="!SELL!",$G$3/G17,0)</f>
+        <v/>
       </c>
       <c r="AE17" s="159" t="n"/>
       <c r="AF17" s="160" t="n"/>
@@ -12695,7 +12778,7 @@
       <c r="D18" s="137" t="n"/>
       <c r="E18" s="138" t="inlineStr">
         <is>
-          <t>06/19</t>
+          <t>05/31</t>
         </is>
       </c>
       <c r="F18" s="139" t="inlineStr">
@@ -12704,86 +12787,94 @@
         </is>
       </c>
       <c r="G18" s="1646" t="n">
-        <v>439.56</v>
+        <v>416.88</v>
       </c>
       <c r="H18" s="1647" t="n">
-        <v>397.21</v>
+        <v>384.64</v>
       </c>
       <c r="I18" s="1648" t="n">
-        <v>354.25</v>
+        <v>351.05</v>
       </c>
       <c r="J18" s="1647" t="n">
-        <v>441.74</v>
+        <v>418.17</v>
       </c>
       <c r="K18" s="1648" t="n">
-        <v>440.59</v>
+        <v>419.66</v>
       </c>
       <c r="L18" s="1647" t="n">
-        <v>440.29</v>
+        <v>418.13</v>
       </c>
       <c r="M18" s="1648" t="n">
-        <v>441.7</v>
-      </c>
-      <c r="N18" s="147" t="inlineStr">
-        <is>
-          <t>HOLD</t>
-        </is>
-      </c>
-      <c r="O18" s="169" t="n">
-        <v>0</v>
-      </c>
-      <c r="P18" s="1661" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q18" s="1695" t="n">
-        <v>2.79</v>
-      </c>
-      <c r="R18" s="238" t="inlineStr">
-        <is>
-          <t>!SELL!</t>
-        </is>
-      </c>
-      <c r="S18" s="239" t="n">
-        <v>2</v>
-      </c>
-      <c r="T18" s="1696" t="n">
-        <v>833.76</v>
-      </c>
-      <c r="U18" s="1697" t="n">
-        <v>1.24</v>
-      </c>
-      <c r="V18" s="151" t="inlineStr">
-        <is>
-          <t>FALSEFALSEFALSE</t>
-        </is>
-      </c>
-      <c r="W18" s="152" t="inlineStr">
-        <is>
-          <t>TRUETRUETRUE</t>
-        </is>
-      </c>
-      <c r="X18" s="1669" t="n">
-        <v>419.67</v>
-      </c>
-      <c r="Y18" s="1670" t="n">
-        <v>418.12</v>
-      </c>
-      <c r="Z18" s="1698" t="n">
-        <v>384.65</v>
-      </c>
-      <c r="AA18" s="1699" t="n">
-        <v>418.12</v>
+        <v>418.24</v>
+      </c>
+      <c r="N18" s="147">
+        <f>IF($V18="TRUETRUETRUE","(!BUY!)","HOLD")</f>
+        <v/>
+      </c>
+      <c r="O18" s="169">
+        <f>ROUNDDOWN($AC18,0)</f>
+        <v/>
+      </c>
+      <c r="P18" s="1661">
+        <f>$O18*$G18</f>
+        <v/>
+      </c>
+      <c r="Q18" s="1695">
+        <f>MAX(J18:M18)-G18+0.01</f>
+        <v/>
+      </c>
+      <c r="R18" s="238">
+        <f>IF(W18="TRUETRUETRUE","!SELL!","HOLD")</f>
+        <v/>
+      </c>
+      <c r="S18" s="239">
+        <f>ROUNDDOWN(AD18,0)</f>
+        <v/>
+      </c>
+      <c r="T18" s="1696">
+        <f>S18*G18</f>
+        <v/>
+      </c>
+      <c r="U18" s="1697">
+        <f>MIN(J18:M18)-G18-0.01</f>
+        <v/>
+      </c>
+      <c r="V18" s="151">
+        <f>IF($G18&lt;$H18,$G18&lt;$I18)&amp;IF($G18&gt;$J18,$G18&gt;$K18)&amp;IF($G18&gt;$L18,$G18&gt;$M18)</f>
+        <v/>
+      </c>
+      <c r="W18" s="152">
+        <f>IF($G18&gt;$H18,$G18&gt;$I18)&amp;IF($G18&lt;$J18,$G18&lt;$K18)&amp;IF($G18&lt;$L18,$G18&lt;$M18)</f>
+        <v/>
+      </c>
+      <c r="X18" s="1669">
+        <f>IF(MAXA(H18:M18)&gt;MINA(H18:I18),MAXA(J18:M18))+0.01</f>
+        <v/>
+      </c>
+      <c r="Y18" s="1670">
+        <f>IF(MINA($H18:$I18)&gt;MAXA($J18:$M18),MINA($H18:$I18),MINA($J18:$M18))-0.01</f>
+        <v/>
+      </c>
+      <c r="Z18" s="1698">
+        <f>MAX(H18,I18)+0.01</f>
+        <v/>
+      </c>
+      <c r="AA18" s="1699">
+        <f>IF(MINA($H18:$I18)&gt;MAXA($J18:$M18),MINA($H18:$I18),MINA($J18:$M18))-0.01</f>
+        <v/>
       </c>
       <c r="AB18" s="157" t="inlineStr">
         <is>
           <t>VGT</t>
         </is>
       </c>
-      <c r="AC18" s="1657" t="n">
-        <v>0</v>
-      </c>
-      <c r="AD18" s="1657" t="n">
-        <v>2.39877182882364</v>
+      <c r="AC18" s="1657">
+        <f>IF(N18="(!BUY!)",$G$3/G18,0)</f>
+        <v/>
+      </c>
+      <c r="AD18" s="1657">
+        <f>IF(R18="!SELL!",$G$3/G18,0)</f>
+        <v/>
       </c>
       <c r="AE18" s="159" t="n"/>
       <c r="AF18" s="160" t="n"/>
@@ -12818,7 +12909,7 @@
       <c r="D19" s="137" t="n"/>
       <c r="E19" s="138" t="inlineStr">
         <is>
-          <t>06/19</t>
+          <t>05/31</t>
         </is>
       </c>
       <c r="F19" s="139" t="inlineStr">
@@ -12827,86 +12918,94 @@
         </is>
       </c>
       <c r="G19" s="1646" t="n">
-        <v>179.37</v>
+        <v>164.74</v>
       </c>
       <c r="H19" s="1647" t="n">
-        <v>174.04</v>
+        <v>173.57</v>
       </c>
       <c r="I19" s="1648" t="n">
-        <v>172.13</v>
+        <v>172.09</v>
       </c>
       <c r="J19" s="1647" t="n">
-        <v>179.02</v>
+        <v>165.04</v>
       </c>
       <c r="K19" s="1648" t="n">
-        <v>178.52</v>
+        <v>166.45</v>
       </c>
       <c r="L19" s="1647" t="n">
-        <v>178.92</v>
+        <v>164.86</v>
       </c>
       <c r="M19" s="1648" t="n">
-        <v>178.68</v>
-      </c>
-      <c r="N19" s="143" t="inlineStr">
-        <is>
-          <t>HOLD</t>
-        </is>
-      </c>
-      <c r="O19" s="144" t="n">
-        <v>0</v>
-      </c>
-      <c r="P19" s="1649" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q19" s="1650" t="n">
-        <v>1.72</v>
-      </c>
-      <c r="R19" s="147" t="inlineStr">
-        <is>
-          <t>HOLD</t>
-        </is>
-      </c>
-      <c r="S19" s="148" t="n">
-        <v>0</v>
-      </c>
-      <c r="T19" s="1651" t="n">
-        <v>0</v>
-      </c>
-      <c r="U19" s="1652" t="n">
-        <v>0.11</v>
-      </c>
-      <c r="V19" s="151" t="inlineStr">
-        <is>
-          <t>TRUEFALSEFALSE</t>
-        </is>
-      </c>
-      <c r="W19" s="152" t="inlineStr">
-        <is>
-          <t>FALSETRUETRUE</t>
-        </is>
-      </c>
-      <c r="X19" s="1701" t="n">
-        <v>166.46</v>
-      </c>
-      <c r="Y19" s="1702" t="n">
-        <v>172.08</v>
-      </c>
-      <c r="Z19" s="1669" t="n">
-        <v>173.58</v>
-      </c>
-      <c r="AA19" s="1670" t="n">
-        <v>172.08</v>
+        <v>166.2</v>
+      </c>
+      <c r="N19" s="143">
+        <f>IF($V19="TRUETRUETRUE","(!BUY!)","HOLD")</f>
+        <v/>
+      </c>
+      <c r="O19" s="144">
+        <f>ROUNDDOWN($AC19,0)</f>
+        <v/>
+      </c>
+      <c r="P19" s="1649">
+        <f>$O19*$G19</f>
+        <v/>
+      </c>
+      <c r="Q19" s="1650">
+        <f>MAX(J19:M19)-G19+0.01</f>
+        <v/>
+      </c>
+      <c r="R19" s="147">
+        <f>IF(W19="TRUETRUETRUE","!SELL!","HOLD")</f>
+        <v/>
+      </c>
+      <c r="S19" s="148">
+        <f>ROUNDDOWN(AD19,0)</f>
+        <v/>
+      </c>
+      <c r="T19" s="1651">
+        <f>S19*G19</f>
+        <v/>
+      </c>
+      <c r="U19" s="1652">
+        <f>MIN(J19:M19)-G19-0.01</f>
+        <v/>
+      </c>
+      <c r="V19" s="151">
+        <f>IF($G19&lt;$H19,$G19&lt;$I19)&amp;IF($G19&gt;$J19,$G19&gt;$K19)&amp;IF($G19&gt;$L19,$G19&gt;$M19)</f>
+        <v/>
+      </c>
+      <c r="W19" s="152">
+        <f>IF($G19&gt;$H19,$G19&gt;$I19)&amp;IF($G19&lt;$J19,$G19&lt;$K19)&amp;IF($G19&lt;$L19,$G19&lt;$M19)</f>
+        <v/>
+      </c>
+      <c r="X19" s="1701">
+        <f>IF(MAXA(H19:M19)&gt;MINA(H19:I19),MAXA(J19:M19))+0.01</f>
+        <v/>
+      </c>
+      <c r="Y19" s="1702">
+        <f>IF(MINA($H19:$I19)&gt;MAXA($J19:$M19),MINA($H19:$I19),MINA($J19:$M19))-0.01</f>
+        <v/>
+      </c>
+      <c r="Z19" s="1669">
+        <f>MAX(H19,I19)+0.01</f>
+        <v/>
+      </c>
+      <c r="AA19" s="1670">
+        <f>IF(MINA($H19:$I19)&gt;MAXA($J19:$M19),MINA($H19:$I19),MINA($J19:$M19))-0.01</f>
+        <v/>
       </c>
       <c r="AB19" s="157" t="inlineStr">
         <is>
           <t>VAW</t>
         </is>
       </c>
-      <c r="AC19" s="1657" t="n">
-        <v>0</v>
-      </c>
-      <c r="AD19" s="1657" t="n">
-        <v>0</v>
+      <c r="AC19" s="1657">
+        <f>IF(N19="(!BUY!)",$G$3/G19,0)</f>
+        <v/>
+      </c>
+      <c r="AD19" s="1657">
+        <f>IF(R19="!SELL!",$G$3/G19,0)</f>
+        <v/>
       </c>
       <c r="AE19" s="159" t="n"/>
       <c r="AF19" s="160" t="n"/>
@@ -12994,7 +13093,7 @@
       <c r="D21" s="137" t="n"/>
       <c r="E21" s="138" t="inlineStr">
         <is>
-          <t>06/19</t>
+          <t>05/31</t>
         </is>
       </c>
       <c r="F21" s="139" t="inlineStr">
@@ -13003,86 +13102,94 @@
         </is>
       </c>
       <c r="G21" s="1706" t="n">
-        <v>83.92</v>
+        <v>80</v>
       </c>
       <c r="H21" s="1707" t="n">
-        <v>81.83</v>
+        <v>81.26000000000001</v>
       </c>
       <c r="I21" s="1708" t="n">
-        <v>84.20999999999999</v>
+        <v>85.14</v>
       </c>
       <c r="J21" s="1707" t="n">
-        <v>84.02</v>
+        <v>79.84</v>
       </c>
       <c r="K21" s="1708" t="n">
-        <v>83.75</v>
+        <v>79.56999999999999</v>
       </c>
       <c r="L21" s="1707" t="n">
-        <v>83.91</v>
+        <v>79.98999999999999</v>
       </c>
       <c r="M21" s="1708" t="n">
-        <v>84</v>
-      </c>
-      <c r="N21" s="227" t="inlineStr">
-        <is>
-          <t>(!BUY!)</t>
-        </is>
-      </c>
-      <c r="O21" s="228" t="n">
-        <v>12</v>
-      </c>
-      <c r="P21" s="1688" t="n">
-        <v>960</v>
-      </c>
-      <c r="Q21" s="1689" t="n">
-        <v>2.08166817117217e-19</v>
-      </c>
-      <c r="R21" s="147" t="inlineStr">
-        <is>
-          <t>HOLD</t>
-        </is>
-      </c>
-      <c r="S21" s="148" t="n">
-        <v>0</v>
-      </c>
-      <c r="T21" s="1661" t="n">
-        <v>0</v>
-      </c>
-      <c r="U21" s="1652" t="n">
-        <v>-0.44</v>
-      </c>
-      <c r="V21" s="151" t="inlineStr">
-        <is>
-          <t>TRUETRUETRUE</t>
-        </is>
-      </c>
-      <c r="W21" s="152" t="inlineStr">
-        <is>
-          <t>FALSEFALSEFALSE</t>
-        </is>
-      </c>
-      <c r="X21" s="1709" t="n">
-        <v>80</v>
-      </c>
-      <c r="Y21" s="1710" t="n">
-        <v>81.25</v>
-      </c>
-      <c r="Z21" s="1655" t="n">
-        <v>85.15000000000001</v>
-      </c>
-      <c r="AA21" s="1656" t="n">
-        <v>81.25</v>
+        <v>79.89</v>
+      </c>
+      <c r="N21" s="227">
+        <f>IF($V21="TRUETRUETRUE","(!BUY!)","HOLD")</f>
+        <v/>
+      </c>
+      <c r="O21" s="228">
+        <f>ROUNDDOWN($AC21,0)</f>
+        <v/>
+      </c>
+      <c r="P21" s="1688">
+        <f>$O21*$G21</f>
+        <v/>
+      </c>
+      <c r="Q21" s="1689">
+        <f>MAX(J21:M21)-G21+0.01</f>
+        <v/>
+      </c>
+      <c r="R21" s="147">
+        <f>IF(W21="TRUETRUETRUE","!SELL!","HOLD")</f>
+        <v/>
+      </c>
+      <c r="S21" s="148">
+        <f>ROUNDDOWN(AD21,0)</f>
+        <v/>
+      </c>
+      <c r="T21" s="1661">
+        <f>S21*G21</f>
+        <v/>
+      </c>
+      <c r="U21" s="1652">
+        <f>MIN(J21:M21)-G21-0.01</f>
+        <v/>
+      </c>
+      <c r="V21" s="151">
+        <f>IF($G21&lt;$H21,$G21&lt;$I21)&amp;IF($G21&gt;$J21,$G21&gt;$K21)&amp;IF($G21&gt;$L21,$G21&gt;$M21)</f>
+        <v/>
+      </c>
+      <c r="W21" s="152">
+        <f>IF($G21&gt;$H21,$G21&gt;$I21)&amp;IF($G21&lt;$J21,$G21&lt;$K21)&amp;IF($G21&lt;$L21,$G21&lt;$M21)</f>
+        <v/>
+      </c>
+      <c r="X21" s="1709">
+        <f>IF(MAXA(H21:M21)&gt;MINA(H21:I21),MAXA(J21:M21))+0.01</f>
+        <v/>
+      </c>
+      <c r="Y21" s="1710">
+        <f>IF(MINA($H21:$I21)&gt;MAXA($J21:$M21),MINA($H21:$I21),MINA($J21:$M21))-0.01</f>
+        <v/>
+      </c>
+      <c r="Z21" s="1655">
+        <f>MAX(H21,I21)+0.01</f>
+        <v/>
+      </c>
+      <c r="AA21" s="1656">
+        <f>IF(MINA($H$21:$I$21)&gt;MAXA($J$21:$M$21),MINA($H$21:$I$21),MINA($J$21:$M$21))-0.01</f>
+        <v/>
       </c>
       <c r="AB21" s="157" t="inlineStr">
         <is>
           <t>VNQ</t>
         </is>
       </c>
-      <c r="AC21" s="1657" t="n">
-        <v>12.5</v>
-      </c>
-      <c r="AD21" s="1657" t="n">
-        <v>0</v>
+      <c r="AC21" s="1657">
+        <f>IF(N21="(!BUY!)",$G$3/G21,0)</f>
+        <v/>
+      </c>
+      <c r="AD21" s="1657">
+        <f>IF(R21="!SELL!",$G$3/G21,0)</f>
+        <v/>
       </c>
       <c r="AE21" s="159" t="n"/>
       <c r="AF21" s="160" t="n"/>
@@ -13116,7 +13223,7 @@
       <c r="D22" s="137" t="n"/>
       <c r="E22" s="138" t="inlineStr">
         <is>
-          <t>06/19</t>
+          <t>05/31</t>
         </is>
       </c>
       <c r="F22" s="139" t="inlineStr">
@@ -13125,86 +13232,94 @@
         </is>
       </c>
       <c r="G22" s="1706" t="n">
-        <v>405.25</v>
+        <v>383.89</v>
       </c>
       <c r="H22" s="1707" t="n">
-        <v>383.44</v>
+        <v>376.74</v>
       </c>
       <c r="I22" s="1708" t="n">
-        <v>365.42</v>
+        <v>364.6</v>
       </c>
       <c r="J22" s="1707" t="n">
-        <v>406.7</v>
+        <v>383.83</v>
       </c>
       <c r="K22" s="1708" t="n">
-        <v>404.96</v>
+        <v>385.12</v>
       </c>
       <c r="L22" s="1707" t="n">
-        <v>405.67</v>
+        <v>384.27</v>
       </c>
       <c r="M22" s="1708" t="n">
-        <v>406.61</v>
-      </c>
-      <c r="N22" s="147" t="inlineStr">
-        <is>
-          <t>HOLD</t>
-        </is>
-      </c>
-      <c r="O22" s="169" t="n">
-        <v>0</v>
-      </c>
-      <c r="P22" s="1661" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q22" s="1662" t="n">
-        <v>1.24</v>
-      </c>
-      <c r="R22" s="179" t="inlineStr">
-        <is>
-          <t>HOLD</t>
-        </is>
-      </c>
-      <c r="S22" s="180" t="n">
-        <v>0</v>
-      </c>
-      <c r="T22" s="1713" t="n">
-        <v>0</v>
-      </c>
-      <c r="U22" s="1668" t="n">
-        <v>-0.07000000000000001</v>
-      </c>
-      <c r="V22" s="151" t="inlineStr">
-        <is>
-          <t>FALSEFALSEFALSE</t>
-        </is>
-      </c>
-      <c r="W22" s="152" t="inlineStr">
-        <is>
-          <t>TRUEFALSETRUE</t>
-        </is>
-      </c>
-      <c r="X22" s="1669" t="n">
-        <v>385.13</v>
-      </c>
-      <c r="Y22" s="1670" t="n">
-        <v>383.82</v>
-      </c>
-      <c r="Z22" s="1671" t="n">
-        <v>376.75</v>
-      </c>
-      <c r="AA22" s="1672" t="n">
-        <v>383.82</v>
+        <v>384</v>
+      </c>
+      <c r="N22" s="147">
+        <f>IF($V22="TRUETRUETRUE","(!BUY!)","HOLD")</f>
+        <v/>
+      </c>
+      <c r="O22" s="169">
+        <f>ROUNDDOWN($AC22,0)</f>
+        <v/>
+      </c>
+      <c r="P22" s="1661">
+        <f>$O22*$G22</f>
+        <v/>
+      </c>
+      <c r="Q22" s="1662">
+        <f>MAX(J22:M22)-G22+0.01</f>
+        <v/>
+      </c>
+      <c r="R22" s="179">
+        <f>IF(W22="TRUETRUETRUE","!SELL!","HOLD")</f>
+        <v/>
+      </c>
+      <c r="S22" s="180">
+        <f>ROUNDDOWN(AD22,0)</f>
+        <v/>
+      </c>
+      <c r="T22" s="1713">
+        <f>S22*G22</f>
+        <v/>
+      </c>
+      <c r="U22" s="1668">
+        <f>MIN(J22:M22)-G22-0.01</f>
+        <v/>
+      </c>
+      <c r="V22" s="151">
+        <f>IF($G22&lt;$H22,$G22&lt;$I22)&amp;IF($G22&gt;$J22,$G22&gt;$K22)&amp;IF($G22&gt;$L22,$G22&gt;$M22)</f>
+        <v/>
+      </c>
+      <c r="W22" s="152">
+        <f>IF($G22&gt;$H22,$G22&gt;$I22)&amp;IF($G22&lt;$J22,$G22&lt;$K22)&amp;IF($G22&lt;$L22,$G22&lt;$M22)</f>
+        <v/>
+      </c>
+      <c r="X22" s="1669">
+        <f>IF(MAXA(H22:M22)&gt;MINA(H22:I22),MAXA(J22:M22))+0.01</f>
+        <v/>
+      </c>
+      <c r="Y22" s="1670">
+        <f>IF(MINA($H22:$I22)&gt;MAXA($J22:$M22),MINA($H22:$I22),MINA($J22:$M22))-0.01</f>
+        <v/>
+      </c>
+      <c r="Z22" s="1671">
+        <f>MAX(H22,I22)+0.01</f>
+        <v/>
+      </c>
+      <c r="AA22" s="1672">
+        <f>IF(MINA($H$22:$I$22)&gt;MAXA($J$22:$M$22),MINA($H$22:$I$22),MINA($J$22:$M$22))-0.01</f>
+        <v/>
       </c>
       <c r="AB22" s="157" t="inlineStr">
         <is>
           <t>VOO</t>
         </is>
       </c>
-      <c r="AC22" s="1657" t="n">
-        <v>0</v>
-      </c>
-      <c r="AD22" s="1657" t="n">
-        <v>0</v>
+      <c r="AC22" s="1657">
+        <f>IF(N22="(!BUY!)",$G$3/G22,0)</f>
+        <v/>
+      </c>
+      <c r="AD22" s="1657">
+        <f>IF(R22="!SELL!",$G$3/G22,0)</f>
+        <v/>
       </c>
       <c r="AE22" s="159" t="n"/>
       <c r="AF22" s="160" t="n"/>
@@ -13238,7 +13353,7 @@
       <c r="D23" s="137" t="n"/>
       <c r="E23" s="138" t="inlineStr">
         <is>
-          <t>06/19</t>
+          <t>05/31</t>
         </is>
       </c>
       <c r="F23" s="139" t="inlineStr">
@@ -13247,86 +13362,94 @@
         </is>
       </c>
       <c r="G23" s="1706" t="n">
-        <v>106.2</v>
+        <v>101.49</v>
       </c>
       <c r="H23" s="1714" t="n">
-        <v>99.64</v>
+        <v>97.39</v>
       </c>
       <c r="I23" s="1715" t="n">
-        <v>91.39</v>
+        <v>91.06999999999999</v>
       </c>
       <c r="J23" s="1716" t="n">
-        <v>106.51</v>
+        <v>101.37</v>
       </c>
       <c r="K23" s="1708" t="n">
-        <v>106.08</v>
+        <v>101.44</v>
       </c>
       <c r="L23" s="1707" t="n">
-        <v>106.32</v>
+        <v>101.49</v>
       </c>
       <c r="M23" s="1708" t="n">
-        <v>106.59</v>
-      </c>
-      <c r="N23" s="147" t="inlineStr">
-        <is>
-          <t>HOLD</t>
-        </is>
-      </c>
-      <c r="O23" s="169" t="n">
-        <v>0</v>
-      </c>
-      <c r="P23" s="1661" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q23" s="1662" t="n">
-        <v>0.01</v>
-      </c>
-      <c r="R23" s="179" t="inlineStr">
-        <is>
-          <t>HOLD</t>
-        </is>
-      </c>
-      <c r="S23" s="180" t="n">
-        <v>0</v>
-      </c>
-      <c r="T23" s="1713" t="n">
-        <v>0</v>
-      </c>
-      <c r="U23" s="1717" t="n">
-        <v>-0.14</v>
-      </c>
-      <c r="V23" s="151" t="inlineStr">
-        <is>
-          <t>FALSETRUEFALSE</t>
-        </is>
-      </c>
-      <c r="W23" s="152" t="inlineStr">
-        <is>
-          <t>TRUEFALSEFALSE</t>
-        </is>
-      </c>
-      <c r="X23" s="1718" t="n">
-        <v>101.5</v>
-      </c>
-      <c r="Y23" s="1719" t="n">
-        <v>101.35</v>
-      </c>
-      <c r="Z23" s="1720" t="n">
-        <v>97.40000000000001</v>
-      </c>
-      <c r="AA23" s="1721" t="n">
-        <v>101.35</v>
+        <v>101.36</v>
+      </c>
+      <c r="N23" s="147">
+        <f>IF($V23="TRUETRUETRUE","(!BUY!)","HOLD")</f>
+        <v/>
+      </c>
+      <c r="O23" s="169">
+        <f>ROUNDDOWN($AC23,0)</f>
+        <v/>
+      </c>
+      <c r="P23" s="1661">
+        <f>$O23*$G23</f>
+        <v/>
+      </c>
+      <c r="Q23" s="1662">
+        <f>MAX(J23:M23)-G23+0.01</f>
+        <v/>
+      </c>
+      <c r="R23" s="179">
+        <f>IF(W23="TRUETRUETRUE","!SELL!","HOLD")</f>
+        <v/>
+      </c>
+      <c r="S23" s="180">
+        <f>ROUNDDOWN(AD23,0)</f>
+        <v/>
+      </c>
+      <c r="T23" s="1713">
+        <f>S23*G23</f>
+        <v/>
+      </c>
+      <c r="U23" s="1717">
+        <f>MIN(J23:M23)-G23-0.01</f>
+        <v/>
+      </c>
+      <c r="V23" s="151">
+        <f>IF($G23&lt;$H23,$G23&lt;$I23)&amp;IF($G23&gt;$J23,$G23&gt;$K23)&amp;IF($G23&gt;$L23,$G23&gt;$M23)</f>
+        <v/>
+      </c>
+      <c r="W23" s="152">
+        <f>IF($G23&gt;$H23,$G23&gt;$I23)&amp;IF($G23&lt;$J23,$G23&lt;$K23)&amp;IF($G23&lt;$L23,$G23&lt;$M23)</f>
+        <v/>
+      </c>
+      <c r="X23" s="1718">
+        <f>IF(MAXA(H23:M23)&gt;MINA(H23:I23),MAXA(J23:M23))+0.01</f>
+        <v/>
+      </c>
+      <c r="Y23" s="1719">
+        <f>IF(MINA($H23:$I23)&gt;MAXA($J23:$M23),MINA($H23:$I23),MINA($J23:$M23))-0.01</f>
+        <v/>
+      </c>
+      <c r="Z23" s="1720">
+        <f>MAX(H23,I23)+0.01</f>
+        <v/>
+      </c>
+      <c r="AA23" s="1721">
+        <f>IF(MINA($H$23:$I$23)&gt;MAXA($J$23:$M$23),MINA($I$23:$J$23),MINA($J$23:$M$23))-0.01</f>
+        <v/>
       </c>
       <c r="AB23" s="157" t="inlineStr">
         <is>
           <t>VOX</t>
         </is>
       </c>
-      <c r="AC23" s="1657" t="n">
-        <v>0</v>
-      </c>
-      <c r="AD23" s="1657" t="n">
-        <v>0</v>
+      <c r="AC23" s="1657">
+        <f>IF(N23="(!BUY!)",$G$3/G23,0)</f>
+        <v/>
+      </c>
+      <c r="AD23" s="1657">
+        <f>IF(R23="!SELL!",$G$3/G23,0)</f>
+        <v/>
       </c>
       <c r="AE23" s="159" t="n"/>
       <c r="AF23" s="160" t="n"/>
@@ -13358,7 +13481,7 @@
       <c r="D24" s="137" t="n"/>
       <c r="E24" s="138" t="inlineStr">
         <is>
-          <t>06/19</t>
+          <t>05/31</t>
         </is>
       </c>
       <c r="F24" s="139" t="inlineStr">
@@ -13367,86 +13490,94 @@
         </is>
       </c>
       <c r="G24" s="1706" t="n">
-        <v>72.73</v>
+        <v>73.04000000000001</v>
       </c>
       <c r="H24" s="1707" t="n">
-        <v>73.28</v>
+        <v>73.55</v>
       </c>
       <c r="I24" s="1708" t="n">
+        <v>72.87</v>
+      </c>
+      <c r="J24" s="1707" t="n">
+        <v>72.98</v>
+      </c>
+      <c r="K24" s="1708" t="n">
         <v>72.7</v>
       </c>
-      <c r="J24" s="1707" t="n">
-        <v>72.7</v>
-      </c>
-      <c r="K24" s="1708" t="n">
-        <v>72.69</v>
-      </c>
       <c r="L24" s="1707" t="n">
-        <v>72.73</v>
+        <v>73.06</v>
       </c>
       <c r="M24" s="1708" t="n">
-        <v>72.70999999999999</v>
-      </c>
-      <c r="N24" s="147" t="inlineStr">
-        <is>
-          <t>HOLD</t>
-        </is>
-      </c>
-      <c r="O24" s="169" t="n">
-        <v>0</v>
-      </c>
-      <c r="P24" s="1661" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q24" s="1662" t="n">
-        <v>0.03</v>
-      </c>
-      <c r="R24" s="147" t="inlineStr">
-        <is>
-          <t>HOLD</t>
-        </is>
-      </c>
-      <c r="S24" s="148" t="n">
-        <v>0</v>
-      </c>
-      <c r="T24" s="1661" t="n">
-        <v>0</v>
-      </c>
-      <c r="U24" s="1722" t="n">
-        <v>-0.35</v>
-      </c>
-      <c r="V24" s="151" t="inlineStr">
-        <is>
-          <t>FALSETRUEFALSE</t>
-        </is>
-      </c>
-      <c r="W24" s="152" t="inlineStr">
-        <is>
-          <t>FALSEFALSEFALSE</t>
-        </is>
-      </c>
-      <c r="X24" s="1655" t="n">
-        <v>73.06999999999999</v>
-      </c>
-      <c r="Y24" s="1656" t="n">
-        <v>72.69</v>
-      </c>
-      <c r="Z24" s="1655" t="n">
-        <v>73.56</v>
-      </c>
-      <c r="AA24" s="1656" t="n">
-        <v>72.69</v>
+        <v>73.01000000000001</v>
+      </c>
+      <c r="N24" s="147">
+        <f>IF($V24="TRUETRUETRUE","(!BUY!)","HOLD")</f>
+        <v/>
+      </c>
+      <c r="O24" s="169">
+        <f>ROUNDDOWN($AC24,0)</f>
+        <v/>
+      </c>
+      <c r="P24" s="1661">
+        <f>$O24*$G24</f>
+        <v/>
+      </c>
+      <c r="Q24" s="1662">
+        <f>MAX(J24:M24)-G24+0.01</f>
+        <v/>
+      </c>
+      <c r="R24" s="147">
+        <f>IF(W24="TRUETRUETRUE","!SELL!","HOLD")</f>
+        <v/>
+      </c>
+      <c r="S24" s="148">
+        <f>ROUNDDOWN(AD24,0)</f>
+        <v/>
+      </c>
+      <c r="T24" s="1661">
+        <f>S24*G24</f>
+        <v/>
+      </c>
+      <c r="U24" s="1722">
+        <f>MIN(J24:M24)-G24-0.01</f>
+        <v/>
+      </c>
+      <c r="V24" s="151">
+        <f>IF($G24&lt;$H24,$G24&lt;$I24)&amp;IF($G24&gt;$J24,$G24&gt;$K24)&amp;IF($G24&gt;$L24,$G24&gt;$M24)</f>
+        <v/>
+      </c>
+      <c r="W24" s="152">
+        <f>IF($G24&gt;$H24,$G24&gt;$I24)&amp;IF($G24&lt;$J24,$G24&lt;$K24)&amp;IF($G24&lt;$L24,$G24&lt;$M24)</f>
+        <v/>
+      </c>
+      <c r="X24" s="1655">
+        <f>IF(MAXA(H24:M24)&gt;MINA(H24:I24),MAXA(J24:M24))+0.01</f>
+        <v/>
+      </c>
+      <c r="Y24" s="1656">
+        <f>IF(MINA($H24:$I24)&gt;MAXA($J24:$M24),MINA($H24:$I24),MINA($J24:$M24))-0.01</f>
+        <v/>
+      </c>
+      <c r="Z24" s="1655">
+        <f>MAX(H24,I24)+0.01</f>
+        <v/>
+      </c>
+      <c r="AA24" s="1656">
+        <f>IF(MINA($H$24:$I$24)&gt;MAXA($J$24:$M$24),MINA($H$24:$I$24),MINA($J$24:$M$24))-0.01</f>
+        <v/>
       </c>
       <c r="AB24" s="157" t="inlineStr">
         <is>
           <t>BND</t>
         </is>
       </c>
-      <c r="AC24" s="1657" t="n">
-        <v>0</v>
-      </c>
-      <c r="AD24" s="1657" t="n">
-        <v>0</v>
+      <c r="AC24" s="1657">
+        <f>IF(N24="(!BUY!)",$G$3/G24,0)</f>
+        <v/>
+      </c>
+      <c r="AD24" s="1657">
+        <f>IF(R24="!SELL!",$G$3/G24,0)</f>
+        <v/>
       </c>
       <c r="AE24" s="159" t="n"/>
       <c r="AF24" s="160" t="n"/>
@@ -13544,7 +13675,7 @@
       <c r="D26" s="137" t="n"/>
       <c r="E26" s="138" t="inlineStr">
         <is>
-          <t>06/19</t>
+          <t>05/31</t>
         </is>
       </c>
       <c r="F26" s="139" t="inlineStr">
@@ -13553,86 +13684,94 @@
         </is>
       </c>
       <c r="G26" s="1646" t="n">
-        <v>48.64</v>
+        <v>48.95</v>
       </c>
       <c r="H26" s="1728" t="n">
-        <v>48.71</v>
+        <v>48.77</v>
       </c>
       <c r="I26" s="1729" t="n">
-        <v>48.43</v>
+        <v>48.52</v>
       </c>
       <c r="J26" s="1728" t="n">
-        <v>48.6</v>
+        <v>48.91</v>
       </c>
       <c r="K26" s="1729" t="n">
-        <v>48.58</v>
+        <v>48.7</v>
       </c>
       <c r="L26" s="1730" t="n">
-        <v>48.61</v>
+        <v>48.94</v>
       </c>
       <c r="M26" s="1731" t="n">
-        <v>48.6</v>
-      </c>
-      <c r="N26" s="147" t="inlineStr">
-        <is>
-          <t>HOLD</t>
-        </is>
-      </c>
-      <c r="O26" s="169" t="n">
-        <v>0</v>
-      </c>
-      <c r="P26" s="1661" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q26" s="1695" t="n">
-        <v>2.08166817117217e-19</v>
-      </c>
-      <c r="R26" s="147" t="inlineStr">
-        <is>
-          <t>HOLD</t>
-        </is>
-      </c>
-      <c r="S26" s="148" t="n">
-        <v>0</v>
-      </c>
-      <c r="T26" s="1651" t="n">
-        <v>0</v>
-      </c>
-      <c r="U26" s="1722" t="n">
-        <v>-0.26</v>
-      </c>
-      <c r="V26" s="151" t="inlineStr">
-        <is>
-          <t>FALSETRUETRUE</t>
-        </is>
-      </c>
-      <c r="W26" s="152" t="inlineStr">
-        <is>
-          <t>TRUEFALSEFALSE</t>
-        </is>
-      </c>
-      <c r="X26" s="1655" t="n">
-        <v>48.95</v>
-      </c>
-      <c r="Y26" s="1656" t="n">
-        <v>48.69</v>
-      </c>
-      <c r="Z26" s="1655" t="n">
-        <v>48.78</v>
-      </c>
-      <c r="AA26" s="1656" t="n">
-        <v>48.69</v>
+        <v>48.92</v>
+      </c>
+      <c r="N26" s="147">
+        <f>IF($V26="TRUETRUETRUE","(!BUY!)","HOLD")</f>
+        <v/>
+      </c>
+      <c r="O26" s="169">
+        <f>ROUNDDOWN($AC26,0)</f>
+        <v/>
+      </c>
+      <c r="P26" s="1661">
+        <f>$O26*$G26</f>
+        <v/>
+      </c>
+      <c r="Q26" s="1695">
+        <f>MAX(J26:M26)-G26+0.01</f>
+        <v/>
+      </c>
+      <c r="R26" s="147">
+        <f>IF(W26="TRUETRUETRUE","!SELL!","HOLD")</f>
+        <v/>
+      </c>
+      <c r="S26" s="148">
+        <f>ROUNDDOWN(AD26,0)</f>
+        <v/>
+      </c>
+      <c r="T26" s="1651">
+        <f>S26*G26</f>
+        <v/>
+      </c>
+      <c r="U26" s="1722">
+        <f>MIN(J26:M26)-G26-0.01</f>
+        <v/>
+      </c>
+      <c r="V26" s="151">
+        <f>IF($G26&lt;$H26,$G26&lt;$I26)&amp;IF($G26&gt;$J26,$G26&gt;$K26)&amp;IF($G26&gt;$L26,$G26&gt;$M26)</f>
+        <v/>
+      </c>
+      <c r="W26" s="152">
+        <f>IF($G26&gt;$H26,$G26&gt;$I26)&amp;IF($G26&lt;$J26,$G26&lt;$K26)&amp;IF($G26&lt;$L26,$G26&lt;$M26)</f>
+        <v/>
+      </c>
+      <c r="X26" s="1655">
+        <f>IF(MAXA(H26:M26)&gt;MINA(H26:I26),MAXA(J26:M26))+0.01</f>
+        <v/>
+      </c>
+      <c r="Y26" s="1656">
+        <f>IF(MINA($H26:$I26)&gt;MAXA($J26:$M26),MINA($H26:$I26),MINA($J26:$M26))-0.01</f>
+        <v/>
+      </c>
+      <c r="Z26" s="1655">
+        <f>MAX(H26,I26)+0.01</f>
+        <v/>
+      </c>
+      <c r="AA26" s="1656">
+        <f>IF(MINA($H$26:$I$26)&gt;MAXA($J$26:$M$26),MINA($H$26:$I$26),MINA($J$26:$M$26))-0.01</f>
+        <v/>
       </c>
       <c r="AB26" s="286" t="inlineStr">
         <is>
           <t>BNDX</t>
         </is>
       </c>
-      <c r="AC26" s="1657" t="n">
-        <v>0</v>
-      </c>
-      <c r="AD26" s="1657" t="n">
-        <v>0</v>
+      <c r="AC26" s="1657">
+        <f>IF(N26="(!BUY!)",$G$3/G26,0)</f>
+        <v/>
+      </c>
+      <c r="AD26" s="1657">
+        <f>IF(R26="!SELL!",$G$3/G26,0)</f>
+        <v/>
       </c>
       <c r="AE26" s="159" t="n"/>
       <c r="AF26" s="160" t="n"/>
@@ -13665,7 +13804,7 @@
       <c r="D27" s="137" t="n"/>
       <c r="E27" s="138" t="inlineStr">
         <is>
-          <t>06/19</t>
+          <t>05/31</t>
         </is>
       </c>
       <c r="F27" s="139" t="inlineStr">
@@ -13674,86 +13813,94 @@
         </is>
       </c>
       <c r="G27" s="1646" t="n">
-        <v>57.62</v>
+        <v>54.28</v>
       </c>
       <c r="H27" s="1647" t="n">
-        <v>55.99</v>
+        <v>55.5</v>
       </c>
       <c r="I27" s="1648" t="n">
-        <v>52.93</v>
+        <v>52.71</v>
       </c>
       <c r="J27" s="1647" t="n">
-        <v>57.72</v>
+        <v>54.12</v>
       </c>
       <c r="K27" s="1648" t="n">
-        <v>57.59</v>
+        <v>54.63</v>
       </c>
       <c r="L27" s="1647" t="n">
-        <v>57.65</v>
+        <v>54.25</v>
       </c>
       <c r="M27" s="1648" t="n">
-        <v>57.73</v>
-      </c>
-      <c r="N27" s="147" t="inlineStr">
-        <is>
-          <t>HOLD</t>
-        </is>
-      </c>
-      <c r="O27" s="169" t="n">
-        <v>0</v>
-      </c>
-      <c r="P27" s="1661" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q27" s="1662" t="n">
-        <v>0.36</v>
-      </c>
-      <c r="R27" s="289" t="inlineStr">
-        <is>
-          <t>HOLD</t>
-        </is>
-      </c>
-      <c r="S27" s="290" t="n">
-        <v>0</v>
-      </c>
-      <c r="T27" s="1733" t="n">
-        <v>0</v>
-      </c>
-      <c r="U27" s="1722" t="n">
-        <v>-0.17</v>
-      </c>
-      <c r="V27" s="151" t="inlineStr">
-        <is>
-          <t>FALSEFALSETRUE</t>
-        </is>
-      </c>
-      <c r="W27" s="152" t="inlineStr">
-        <is>
-          <t>FALSEFALSEFALSE</t>
-        </is>
-      </c>
-      <c r="X27" s="1655" t="n">
-        <v>54.64</v>
-      </c>
-      <c r="Y27" s="1656" t="n">
-        <v>54.11</v>
-      </c>
-      <c r="Z27" s="1655" t="n">
-        <v>55.51</v>
-      </c>
-      <c r="AA27" s="1656" t="n">
-        <v>54.11</v>
+        <v>54.16</v>
+      </c>
+      <c r="N27" s="147">
+        <f>IF($V27="TRUETRUETRUE","(!BUY!)","HOLD")</f>
+        <v/>
+      </c>
+      <c r="O27" s="169">
+        <f>ROUNDDOWN($AC27,0)</f>
+        <v/>
+      </c>
+      <c r="P27" s="1661">
+        <f>$O27*$G27</f>
+        <v/>
+      </c>
+      <c r="Q27" s="1662">
+        <f>MAX(J27:M27)-G27+0.01</f>
+        <v/>
+      </c>
+      <c r="R27" s="289">
+        <f>IF(W27="TRUETRUETRUE","!SELL!","HOLD")</f>
+        <v/>
+      </c>
+      <c r="S27" s="290">
+        <f>ROUNDDOWN(AD27,0)</f>
+        <v/>
+      </c>
+      <c r="T27" s="1733">
+        <f>S27*G27</f>
+        <v/>
+      </c>
+      <c r="U27" s="1722">
+        <f>MIN(J27:M27)-G27-0.01</f>
+        <v/>
+      </c>
+      <c r="V27" s="151">
+        <f>IF($G27&lt;$H27,$G27&lt;$I27)&amp;IF($G27&gt;$J27,$G27&gt;$K27)&amp;IF($G27&gt;$L27,$G27&gt;$M27)</f>
+        <v/>
+      </c>
+      <c r="W27" s="152">
+        <f>IF($G27&gt;$H27,$G27&gt;$I27)&amp;IF($G27&lt;$J27,$G27&lt;$K27)&amp;IF($G27&lt;$L27,$G27&lt;$M27)</f>
+        <v/>
+      </c>
+      <c r="X27" s="1655">
+        <f>IF(MAXA(H27:M27)&gt;MINA(H27:I27),MAXA(J27:M27))+0.01</f>
+        <v/>
+      </c>
+      <c r="Y27" s="1656">
+        <f>IF(MINA($H27:$I27)&gt;MAXA($J27:$M27),MINA($H27:$I27),MINA($J27:$M27))-0.01</f>
+        <v/>
+      </c>
+      <c r="Z27" s="1655">
+        <f>MAX(H27,I27)+0.01</f>
+        <v/>
+      </c>
+      <c r="AA27" s="1656">
+        <f>IF(MINA($H27:$I27)&gt;MAXA($J27:$M27),MINA($H27:$I27),MINA($J27:$M27))-0.01</f>
+        <v/>
       </c>
       <c r="AB27" s="292" t="inlineStr">
         <is>
           <t>VXUS</t>
         </is>
       </c>
-      <c r="AC27" s="1657" t="n">
-        <v>0</v>
-      </c>
-      <c r="AD27" s="1657" t="n">
-        <v>0</v>
+      <c r="AC27" s="1657">
+        <f>IF(N27="(!BUY!)",$G$3/G27,0)</f>
+        <v/>
+      </c>
+      <c r="AD27" s="1657">
+        <f>IF(R27="!SELL!",$G$3/G27,0)</f>
+        <v/>
       </c>
       <c r="AE27" s="159" t="n"/>
       <c r="AF27" s="160" t="n"/>
@@ -13787,7 +13934,7 @@
       <c r="D28" s="137" t="n"/>
       <c r="E28" s="138" t="inlineStr">
         <is>
-          <t>06/19</t>
+          <t>05/31</t>
         </is>
       </c>
       <c r="F28" s="139" t="inlineStr">
@@ -13796,86 +13943,94 @@
         </is>
       </c>
       <c r="G28" s="1646" t="n">
-        <v>219.26</v>
+        <v>207.18</v>
       </c>
       <c r="H28" s="1647" t="n">
-        <v>207.35</v>
+        <v>203.77</v>
       </c>
       <c r="I28" s="1648" t="n">
-        <v>198.92</v>
+        <v>198.59</v>
       </c>
       <c r="J28" s="1647" t="n">
-        <v>219.91</v>
+        <v>207.13</v>
       </c>
       <c r="K28" s="1648" t="n">
-        <v>219.11</v>
+        <v>207.87</v>
       </c>
       <c r="L28" s="1647" t="n">
-        <v>219.43</v>
+        <v>207.39</v>
       </c>
       <c r="M28" s="1648" t="n">
-        <v>219.88</v>
-      </c>
-      <c r="N28" s="147" t="inlineStr">
-        <is>
-          <t>HOLD</t>
-        </is>
-      </c>
-      <c r="O28" s="169" t="n">
-        <v>0</v>
-      </c>
-      <c r="P28" s="1661" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q28" s="1662" t="n">
-        <v>0.7</v>
-      </c>
-      <c r="R28" s="179" t="inlineStr">
-        <is>
-          <t>HOLD</t>
-        </is>
-      </c>
-      <c r="S28" s="180" t="n">
-        <v>0</v>
-      </c>
-      <c r="T28" s="1667" t="n">
-        <v>0</v>
-      </c>
-      <c r="U28" s="1668" t="n">
-        <v>-0.06</v>
-      </c>
-      <c r="V28" s="151" t="inlineStr">
-        <is>
-          <t>FALSEFALSEFALSE</t>
-        </is>
-      </c>
-      <c r="W28" s="152" t="inlineStr">
-        <is>
-          <t>TRUEFALSETRUE</t>
-        </is>
-      </c>
-      <c r="X28" s="1669" t="n">
-        <v>207.88</v>
-      </c>
-      <c r="Y28" s="1670" t="n">
-        <v>207.12</v>
-      </c>
-      <c r="Z28" s="1671" t="n">
-        <v>203.78</v>
-      </c>
-      <c r="AA28" s="1672" t="n">
-        <v>207.12</v>
+        <v>207.23</v>
+      </c>
+      <c r="N28" s="147">
+        <f>IF($V28="TRUETRUETRUE","(!BUY!)","HOLD")</f>
+        <v/>
+      </c>
+      <c r="O28" s="169">
+        <f>ROUNDDOWN($AC28,0)</f>
+        <v/>
+      </c>
+      <c r="P28" s="1661">
+        <f>$O28*$G28</f>
+        <v/>
+      </c>
+      <c r="Q28" s="1662">
+        <f>MAX(J28:M28)-G28+0.01</f>
+        <v/>
+      </c>
+      <c r="R28" s="179">
+        <f>IF(W28="TRUETRUETRUE","!SELL!","HOLD")</f>
+        <v/>
+      </c>
+      <c r="S28" s="180">
+        <f>ROUNDDOWN(AD28,0)</f>
+        <v/>
+      </c>
+      <c r="T28" s="1667">
+        <f>S28*G28</f>
+        <v/>
+      </c>
+      <c r="U28" s="1668">
+        <f>MIN(J28:M28)-G28-0.01</f>
+        <v/>
+      </c>
+      <c r="V28" s="151">
+        <f>IF($G28&lt;$H28,$G28&lt;$I28)&amp;IF($G28&gt;$J28,$G28&gt;$K28)&amp;IF($G28&gt;$L28,$G28&gt;$M28)</f>
+        <v/>
+      </c>
+      <c r="W28" s="152">
+        <f>IF($G28&gt;$H28,$G28&gt;$I28)&amp;IF($G28&lt;$J28,$G28&lt;$K28)&amp;IF($G28&lt;$L28,$G28&lt;$M28)</f>
+        <v/>
+      </c>
+      <c r="X28" s="1669">
+        <f>IF(MAXA(H28:M28)&gt;MINA(H28:I28),MAXA(J28:M28))+0.01</f>
+        <v/>
+      </c>
+      <c r="Y28" s="1670">
+        <f>IF(MINA($H28:$I28)&gt;MAXA($J28:$M28),MINA($H28:$I28),MINA($J28:$M28))-0.01</f>
+        <v/>
+      </c>
+      <c r="Z28" s="1671">
+        <f>MAX(H28,I28)+0.01</f>
+        <v/>
+      </c>
+      <c r="AA28" s="1672">
+        <f>IF(MINA($H28:$I28)&gt;MAXA($J28:$M28),MINA($H28:$I28),MINA($J28:$M28))-0.01</f>
+        <v/>
       </c>
       <c r="AB28" s="157" t="inlineStr">
         <is>
           <t>VTI</t>
         </is>
       </c>
-      <c r="AC28" s="1657" t="n">
-        <v>0</v>
-      </c>
-      <c r="AD28" s="1657" t="n">
-        <v>0</v>
+      <c r="AC28" s="1657">
+        <f>IF(N28="(!BUY!)",$G$3/G28,0)</f>
+        <v/>
+      </c>
+      <c r="AD28" s="1657">
+        <f>IF(R28="!SELL!",$G$3/G28,0)</f>
+        <v/>
       </c>
       <c r="AE28" s="159" t="n"/>
       <c r="AF28" s="160" t="n"/>
@@ -13907,7 +14062,7 @@
       <c r="D29" s="137" t="n"/>
       <c r="E29" s="138" t="inlineStr">
         <is>
-          <t>06/19</t>
+          <t>05/31</t>
         </is>
       </c>
       <c r="F29" s="139" t="inlineStr">
@@ -13916,86 +14071,94 @@
         </is>
       </c>
       <c r="G29" s="1646" t="n">
-        <v>146.24</v>
+        <v>141.32</v>
       </c>
       <c r="H29" s="1647" t="n">
-        <v>146.98</v>
+        <v>147.25</v>
       </c>
       <c r="I29" s="1648" t="n">
-        <v>149.12</v>
+        <v>150.49</v>
       </c>
       <c r="J29" s="1647" t="n">
-        <v>146.74</v>
+        <v>141.18</v>
       </c>
       <c r="K29" s="1648" t="n">
-        <v>145.61</v>
+        <v>140.53</v>
       </c>
       <c r="L29" s="1647" t="n">
-        <v>146.4</v>
+        <v>141.58</v>
       </c>
       <c r="M29" s="1648" t="n">
-        <v>146.67</v>
-      </c>
-      <c r="N29" s="143" t="inlineStr">
-        <is>
-          <t>HOLD</t>
-        </is>
-      </c>
-      <c r="O29" s="144" t="n">
-        <v>0</v>
-      </c>
-      <c r="P29" s="1649" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q29" s="1650" t="n">
-        <v>0.27</v>
-      </c>
-      <c r="R29" s="147" t="inlineStr">
-        <is>
-          <t>HOLD</t>
-        </is>
-      </c>
-      <c r="S29" s="148" t="n">
-        <v>0</v>
-      </c>
-      <c r="T29" s="1651" t="n">
-        <v>0</v>
-      </c>
-      <c r="U29" s="1652" t="n">
-        <v>-0.8</v>
-      </c>
-      <c r="V29" s="151" t="inlineStr">
-        <is>
-          <t>TRUETRUEFALSE</t>
-        </is>
-      </c>
-      <c r="W29" s="152" t="inlineStr">
-        <is>
-          <t>FALSEFALSEFALSE</t>
-        </is>
-      </c>
-      <c r="X29" s="1674" t="n">
-        <v>141.59</v>
-      </c>
-      <c r="Y29" s="1675" t="n">
-        <v>147.24</v>
-      </c>
-      <c r="Z29" s="1669" t="n">
-        <v>150.5</v>
-      </c>
-      <c r="AA29" s="1670" t="n">
-        <v>147.24</v>
+        <v>140.7</v>
+      </c>
+      <c r="N29" s="143">
+        <f>IF($V29="TRUETRUETRUE","(!BUY!)","HOLD")</f>
+        <v/>
+      </c>
+      <c r="O29" s="144">
+        <f>ROUNDDOWN($AC29,0)</f>
+        <v/>
+      </c>
+      <c r="P29" s="1649">
+        <f>$O29*$G29</f>
+        <v/>
+      </c>
+      <c r="Q29" s="1650">
+        <f>MAX(J29:M29)-G29+0.01</f>
+        <v/>
+      </c>
+      <c r="R29" s="147">
+        <f>IF(W29="TRUETRUETRUE","!SELL!","HOLD")</f>
+        <v/>
+      </c>
+      <c r="S29" s="148">
+        <f>ROUNDDOWN(AD29,0)</f>
+        <v/>
+      </c>
+      <c r="T29" s="1651">
+        <f>S29*G29</f>
+        <v/>
+      </c>
+      <c r="U29" s="1652">
+        <f>MIN(J29:M29)-G29-0.01</f>
+        <v/>
+      </c>
+      <c r="V29" s="151">
+        <f>IF($G29&lt;$H29,$G29&lt;$I29)&amp;IF($G29&gt;$J29,$G29&gt;$K29)&amp;IF($G29&gt;$L29,$G29&gt;$M29)</f>
+        <v/>
+      </c>
+      <c r="W29" s="152">
+        <f>IF($G29&gt;$H29,$G29&gt;$I29)&amp;IF($G29&lt;$J29,$G29&lt;$K29)&amp;IF($G29&lt;$L29,$G29&lt;$M29)</f>
+        <v/>
+      </c>
+      <c r="X29" s="1674">
+        <f>IF(MAXA(H29:M29)&gt;MINA(H29:I29),MAXA(J29:M29))+0.01</f>
+        <v/>
+      </c>
+      <c r="Y29" s="1675">
+        <f>IF(MINA($H29:$I29)&gt;MAXA($J29:$M29),MINA($H29:$I29),MINA($J29:$M29))-0.01</f>
+        <v/>
+      </c>
+      <c r="Z29" s="1669">
+        <f>MAX(H29,I29)+0.01</f>
+        <v/>
+      </c>
+      <c r="AA29" s="1670">
+        <f>IF(MINA($H29:$I29)&gt;MAXA($J29:$M29),MINA($H29:$I29),MINA($J29:$M29))-0.01</f>
+        <v/>
       </c>
       <c r="AB29" s="157" t="inlineStr">
         <is>
           <t>VPU</t>
         </is>
       </c>
-      <c r="AC29" s="1657" t="n">
-        <v>0</v>
-      </c>
-      <c r="AD29" s="1657" t="n">
-        <v>0</v>
+      <c r="AC29" s="1657">
+        <f>IF(N29="(!BUY!)",$G$3/G29,0)</f>
+        <v/>
+      </c>
+      <c r="AD29" s="1657">
+        <f>IF(R29="!SELL!",$G$3/G29,0)</f>
+        <v/>
       </c>
       <c r="AE29" s="159" t="n"/>
       <c r="AF29" s="160" t="n"/>
@@ -14029,7 +14192,7 @@
       <c r="D30" s="137" t="n"/>
       <c r="E30" s="138" t="inlineStr">
         <is>
-          <t>06/19</t>
+          <t>05/31</t>
         </is>
       </c>
       <c r="F30" s="139" t="inlineStr">
@@ -14038,86 +14201,94 @@
         </is>
       </c>
       <c r="G30" s="1646" t="n">
-        <v>79.92</v>
+        <v>71.95999999999999</v>
       </c>
       <c r="H30" s="1647" t="n">
-        <v>73.3</v>
+        <v>71.63</v>
       </c>
       <c r="I30" s="1648" t="n">
-        <v>72.18000000000001</v>
+        <v>72.2</v>
       </c>
       <c r="J30" s="1647" t="n">
-        <v>80</v>
+        <v>72.01000000000001</v>
       </c>
       <c r="K30" s="1648" t="n">
-        <v>79.17</v>
+        <v>72.54000000000001</v>
       </c>
       <c r="L30" s="1647" t="n">
-        <v>80.18000000000001</v>
+        <v>72</v>
       </c>
       <c r="M30" s="1648" t="n">
-        <v>79.2</v>
-      </c>
-      <c r="N30" s="147" t="inlineStr">
-        <is>
-          <t>HOLD</t>
-        </is>
-      </c>
-      <c r="O30" s="169" t="n">
-        <v>0</v>
-      </c>
-      <c r="P30" s="1661" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q30" s="1662" t="n">
-        <v>0.62</v>
-      </c>
-      <c r="R30" s="147" t="inlineStr">
-        <is>
-          <t>HOLD</t>
-        </is>
-      </c>
-      <c r="S30" s="148" t="n">
-        <v>0</v>
-      </c>
-      <c r="T30" s="1651" t="n">
-        <v>0</v>
-      </c>
-      <c r="U30" s="1652" t="n">
-        <v>0.03</v>
-      </c>
-      <c r="V30" s="151" t="inlineStr">
-        <is>
-          <t>FALSEFALSEFALSE</t>
-        </is>
-      </c>
-      <c r="W30" s="152" t="inlineStr">
-        <is>
-          <t>FALSETRUETRUE</t>
-        </is>
-      </c>
-      <c r="X30" s="1655" t="n">
-        <v>72.58</v>
-      </c>
-      <c r="Y30" s="1656" t="n">
-        <v>71.98999999999999</v>
-      </c>
-      <c r="Z30" s="1655" t="n">
-        <v>72.20999999999999</v>
-      </c>
-      <c r="AA30" s="1656" t="n">
-        <v>71.98999999999999</v>
+        <v>72.56999999999999</v>
+      </c>
+      <c r="N30" s="147">
+        <f>IF($V30="TRUETRUETRUE","(!BUY!)","HOLD")</f>
+        <v/>
+      </c>
+      <c r="O30" s="169">
+        <f>ROUNDDOWN($AC30,0)</f>
+        <v/>
+      </c>
+      <c r="P30" s="1661">
+        <f>$O30*$G30</f>
+        <v/>
+      </c>
+      <c r="Q30" s="1662">
+        <f>MAX(J30:M30)-G30+0.01</f>
+        <v/>
+      </c>
+      <c r="R30" s="147">
+        <f>IF(W30="TRUETRUETRUE","!SELL!","HOLD")</f>
+        <v/>
+      </c>
+      <c r="S30" s="148">
+        <f>ROUNDDOWN(AD30,0)</f>
+        <v/>
+      </c>
+      <c r="T30" s="1651">
+        <f>S30*G30</f>
+        <v/>
+      </c>
+      <c r="U30" s="1652">
+        <f>MIN(J30:M30)-G30-0.01</f>
+        <v/>
+      </c>
+      <c r="V30" s="151">
+        <f>IF($G30&lt;$H30,$G30&lt;$I30)&amp;IF($G30&gt;$J30,$G30&gt;$K30)&amp;IF($G30&gt;$L30,$G30&gt;$M30)</f>
+        <v/>
+      </c>
+      <c r="W30" s="152">
+        <f>IF($G30&gt;$H30,$G30&gt;$I30)&amp;IF($G30&lt;$J30,$G30&lt;$K30)&amp;IF($G30&lt;$L30,$G30&lt;$M30)</f>
+        <v/>
+      </c>
+      <c r="X30" s="1655">
+        <f>IF(MAXA(H30:M30)&gt;MINA(H30:I30),MAXA(J30:M30))+0.01</f>
+        <v/>
+      </c>
+      <c r="Y30" s="1656">
+        <f>IF(MINA($H30:$I30)&gt;MAXA($J30:$M30),MINA($H30:$I30),MINA($J30:$M30))-0.01</f>
+        <v/>
+      </c>
+      <c r="Z30" s="1655">
+        <f>MAX(H30,I30)+0.01</f>
+        <v/>
+      </c>
+      <c r="AA30" s="1656">
+        <f>IF(MINA($H30:$I30)&gt;MAXA($J30:$M30),MINA($H30:$I30),MINA($J30:$M30))-0.01</f>
+        <v/>
       </c>
       <c r="AB30" s="157" t="inlineStr">
         <is>
           <t>XTN</t>
         </is>
       </c>
-      <c r="AC30" s="1657" t="n">
-        <v>0</v>
-      </c>
-      <c r="AD30" s="1657" t="n">
-        <v>0</v>
+      <c r="AC30" s="1657">
+        <f>IF(N30="(!BUY!)",$G$3/G30,0)</f>
+        <v/>
+      </c>
+      <c r="AD30" s="1657">
+        <f>IF(R30="!SELL!",$G$3/G30,0)</f>
+        <v/>
       </c>
       <c r="AE30" s="159" t="n"/>
       <c r="AF30" s="160" t="n"/>

</xml_diff>

<commit_message>
implemented basic main function (doesn't work)
</commit_message>
<xml_diff>
--- a/src/testPlatform.xlsx
+++ b/src/testPlatform.xlsx
@@ -11373,7 +11373,7 @@
       <c r="D6" s="137" t="n"/>
       <c r="E6" s="138" t="inlineStr">
         <is>
-          <t>06/22</t>
+          <t>06/25</t>
         </is>
       </c>
       <c r="F6" s="139" t="inlineStr">
@@ -11382,25 +11382,25 @@
         </is>
       </c>
       <c r="G6" s="1646" t="n">
-        <v>-1</v>
+        <v>90.90000000000001</v>
       </c>
       <c r="H6" s="1647" t="n">
-        <v>91.54000000000001</v>
+        <v>91.5</v>
       </c>
       <c r="I6" s="1648" t="n">
-        <v>91.18000000000001</v>
+        <v>91.17</v>
       </c>
       <c r="J6" s="1647" t="n">
-        <v>91.93000000000001</v>
+        <v>90.88</v>
       </c>
       <c r="K6" s="1648" t="n">
-        <v>91.93000000000001</v>
+        <v>91.13</v>
       </c>
       <c r="L6" s="1647" t="n">
-        <v>91.90000000000001</v>
+        <v>90.88</v>
       </c>
       <c r="M6" s="1648" t="n">
-        <v>91.93000000000001</v>
+        <v>90.88</v>
       </c>
       <c r="N6" s="143">
         <f>IF($V6="TRUETRUETRUE","(!BUY!)","HOLD")</f>

</xml_diff>

<commit_message>
renamed polygon_data to get_data. Implemented yfinance for close price
</commit_message>
<xml_diff>
--- a/src/testPlatform.xlsx
+++ b/src/testPlatform.xlsx
@@ -11382,25 +11382,25 @@
         </is>
       </c>
       <c r="G6" s="1646" t="n">
-        <v>-1</v>
+        <v>91.34</v>
       </c>
       <c r="H6" s="1647" t="n">
-        <v>91.5</v>
+        <v>91.45</v>
       </c>
       <c r="I6" s="1648" t="n">
-        <v>91.17</v>
+        <v>91.16</v>
       </c>
       <c r="J6" s="1647" t="n">
-        <v>90.88</v>
+        <v>91.34999999999999</v>
       </c>
       <c r="K6" s="1648" t="n">
-        <v>91.13</v>
+        <v>91.09999999999999</v>
       </c>
       <c r="L6" s="1647" t="n">
-        <v>90.88</v>
+        <v>91.31999999999999</v>
       </c>
       <c r="M6" s="1648" t="n">
-        <v>90.88</v>
+        <v>91.36</v>
       </c>
       <c r="N6" s="143">
         <f>IF($V6="TRUETRUETRUE","(!BUY!)","HOLD")</f>
@@ -11508,25 +11508,25 @@
         </is>
       </c>
       <c r="G7" s="1646" t="n">
-        <v>30.31</v>
+        <v>29.65</v>
       </c>
       <c r="H7" s="1647" t="n">
-        <v>33.2</v>
+        <v>32.42</v>
       </c>
       <c r="I7" s="1648" t="n">
-        <v>28.83</v>
+        <v>29.36</v>
       </c>
       <c r="J7" s="1647" t="n">
-        <v>30.94</v>
+        <v>29.53</v>
       </c>
       <c r="K7" s="1648" t="n">
-        <v>30.54</v>
+        <v>29.8</v>
       </c>
       <c r="L7" s="1647" t="n">
-        <v>30.85</v>
+        <v>29.61</v>
       </c>
       <c r="M7" s="1648" t="n">
-        <v>30.92</v>
+        <v>29.53</v>
       </c>
       <c r="N7" s="147">
         <f>IF($V7="TRUETRUETRUE","(!BUY!)","HOLD")</f>
@@ -11636,25 +11636,25 @@
         </is>
       </c>
       <c r="G8" s="1646" t="n">
-        <v>253.25</v>
+        <v>278.78</v>
       </c>
       <c r="H8" s="1647" t="n">
-        <v>248.76</v>
+        <v>258.32</v>
       </c>
       <c r="I8" s="1648" t="n">
-        <v>245.06</v>
+        <v>245.31</v>
       </c>
       <c r="J8" s="1647" t="n">
-        <v>252.73</v>
+        <v>277.19</v>
       </c>
       <c r="K8" s="1648" t="n">
-        <v>253.62</v>
+        <v>276.73</v>
       </c>
       <c r="L8" s="1647" t="n">
-        <v>251.96</v>
+        <v>278.16</v>
       </c>
       <c r="M8" s="1648" t="n">
-        <v>254.78</v>
+        <v>276.25</v>
       </c>
       <c r="N8" s="147">
         <f>IF($V8="TRUETRUETRUE","(!BUY!)","HOLD")</f>

</xml_diff>

<commit_message>
trade ranges are added to the correct etf blocks
</commit_message>
<xml_diff>
--- a/src/testPlatform.xlsx
+++ b/src/testPlatform.xlsx
@@ -11382,25 +11382,25 @@
         </is>
       </c>
       <c r="G6" s="1646" t="n">
-        <v>91.34</v>
+        <v>91.63</v>
       </c>
       <c r="H6" s="1647" t="n">
-        <v>91.45</v>
+        <v>91.43000000000001</v>
       </c>
       <c r="I6" s="1648" t="n">
-        <v>91.16</v>
+        <v>91.14</v>
       </c>
       <c r="J6" s="1647" t="n">
-        <v>91.34999999999999</v>
+        <v>91.51000000000001</v>
       </c>
       <c r="K6" s="1648" t="n">
-        <v>91.09999999999999</v>
+        <v>91.5</v>
       </c>
       <c r="L6" s="1647" t="n">
-        <v>91.31999999999999</v>
+        <v>91.58</v>
       </c>
       <c r="M6" s="1648" t="n">
-        <v>91.36</v>
+        <v>91.51000000000001</v>
       </c>
       <c r="N6" s="143">
         <f>IF($V6="TRUETRUETRUE","(!BUY!)","HOLD")</f>
@@ -11508,25 +11508,25 @@
         </is>
       </c>
       <c r="G7" s="1646" t="n">
-        <v>29.65</v>
+        <v>29.62</v>
       </c>
       <c r="H7" s="1647" t="n">
-        <v>32.42</v>
+        <v>32.22</v>
       </c>
       <c r="I7" s="1648" t="n">
-        <v>29.36</v>
+        <v>29.4</v>
       </c>
       <c r="J7" s="1647" t="n">
-        <v>29.53</v>
+        <v>29.49</v>
       </c>
       <c r="K7" s="1648" t="n">
-        <v>29.8</v>
+        <v>29.39</v>
       </c>
       <c r="L7" s="1647" t="n">
-        <v>29.61</v>
+        <v>29.49</v>
       </c>
       <c r="M7" s="1648" t="n">
-        <v>29.53</v>
+        <v>29.49</v>
       </c>
       <c r="N7" s="147">
         <f>IF($V7="TRUETRUETRUE","(!BUY!)","HOLD")</f>
@@ -11636,25 +11636,25 @@
         </is>
       </c>
       <c r="G8" s="1646" t="n">
-        <v>278.78</v>
+        <v>279.68</v>
       </c>
       <c r="H8" s="1647" t="n">
-        <v>258.32</v>
+        <v>259.48</v>
       </c>
       <c r="I8" s="1648" t="n">
-        <v>245.31</v>
+        <v>245.38</v>
       </c>
       <c r="J8" s="1647" t="n">
-        <v>277.19</v>
+        <v>279.19</v>
       </c>
       <c r="K8" s="1648" t="n">
-        <v>276.73</v>
+        <v>277.63</v>
       </c>
       <c r="L8" s="1647" t="n">
-        <v>278.16</v>
+        <v>279.03</v>
       </c>
       <c r="M8" s="1648" t="n">
-        <v>276.25</v>
+        <v>278.92</v>
       </c>
       <c r="N8" s="147">
         <f>IF($V8="TRUETRUETRUE","(!BUY!)","HOLD")</f>
@@ -11763,25 +11763,25 @@
         </is>
       </c>
       <c r="G9" s="1646" t="n">
-        <v>189.6</v>
+        <v>192.75</v>
       </c>
       <c r="H9" s="1647" t="n">
-        <v>195.25</v>
+        <v>195.46</v>
       </c>
       <c r="I9" s="1648" t="n">
-        <v>190.21</v>
+        <v>190.24</v>
       </c>
       <c r="J9" s="1647" t="n">
-        <v>189.84</v>
+        <v>192.7</v>
       </c>
       <c r="K9" s="1648" t="n">
-        <v>189.94</v>
+        <v>193.81</v>
       </c>
       <c r="L9" s="1647" t="n">
-        <v>190.12</v>
+        <v>192.62</v>
       </c>
       <c r="M9" s="1648" t="n">
-        <v>189.61</v>
+        <v>192.89</v>
       </c>
       <c r="N9" s="143">
         <f>IF($V9="TRUETRUETRUE","(!BUY!)","HOLD")</f>
@@ -11939,25 +11939,25 @@
         </is>
       </c>
       <c r="G11" s="1646" t="n">
-        <v>153.25</v>
+        <v>160.79</v>
       </c>
       <c r="H11" s="1647" t="n">
-        <v>154.47</v>
+        <v>156.8</v>
       </c>
       <c r="I11" s="1648" t="n">
-        <v>151.51</v>
+        <v>152.1</v>
       </c>
       <c r="J11" s="1647" t="n">
-        <v>153.28</v>
+        <v>160.52</v>
       </c>
       <c r="K11" s="1648" t="n">
-        <v>153.8</v>
+        <v>160.31</v>
       </c>
       <c r="L11" s="1647" t="n">
-        <v>153.45</v>
+        <v>160.63</v>
       </c>
       <c r="M11" s="1648" t="n">
-        <v>153.33</v>
+        <v>160.52</v>
       </c>
       <c r="N11" s="147">
         <f>IF($V11="TRUETRUETRUE","(!BUY!)","HOLD")</f>
@@ -12068,25 +12068,25 @@
         </is>
       </c>
       <c r="G12" s="1646" t="n">
-        <v>105.87</v>
+        <v>112.13</v>
       </c>
       <c r="H12" s="1647" t="n">
-        <v>112.95</v>
+        <v>111.22</v>
       </c>
       <c r="I12" s="1648" t="n">
-        <v>117.12</v>
+        <v>116.91</v>
       </c>
       <c r="J12" s="1647" t="n">
-        <v>105.97</v>
+        <v>111.59</v>
       </c>
       <c r="K12" s="1648" t="n">
-        <v>107.13</v>
+        <v>111.14</v>
       </c>
       <c r="L12" s="1647" t="n">
-        <v>105.88</v>
+        <v>111.78</v>
       </c>
       <c r="M12" s="1648" t="n">
-        <v>105.96</v>
+        <v>111.59</v>
       </c>
       <c r="N12" s="143">
         <f>IF($V12="TRUETRUETRUE","(!BUY!)","HOLD")</f>
@@ -12200,25 +12200,25 @@
         </is>
       </c>
       <c r="G13" s="1646" t="n">
-        <v>76.44</v>
+        <v>80.65000000000001</v>
       </c>
       <c r="H13" s="1647" t="n">
-        <v>77.48</v>
+        <v>78.5</v>
       </c>
       <c r="I13" s="1648" t="n">
-        <v>82.09999999999999</v>
+        <v>81.68000000000001</v>
       </c>
       <c r="J13" s="1647" t="n">
-        <v>76.36</v>
+        <v>80.56999999999999</v>
       </c>
       <c r="K13" s="1648" t="n">
-        <v>76.90000000000001</v>
+        <v>80.03</v>
       </c>
       <c r="L13" s="1647" t="n">
-        <v>76.53</v>
+        <v>80.62</v>
       </c>
       <c r="M13" s="1648" t="n">
-        <v>76.34999999999999</v>
+        <v>80.53</v>
       </c>
       <c r="N13" s="143">
         <f>IF($V13="TRUETRUETRUE","(!BUY!)","HOLD")</f>
@@ -12332,25 +12332,25 @@
         </is>
       </c>
       <c r="G14" s="1646" t="n">
-        <v>39.05</v>
+        <v>40.33</v>
       </c>
       <c r="H14" s="1647" t="n">
-        <v>40.04</v>
+        <v>40.25</v>
       </c>
       <c r="I14" s="1648" t="n">
-        <v>39.69</v>
+        <v>39.63</v>
       </c>
       <c r="J14" s="1647" t="n">
-        <v>38.93</v>
+        <v>40.31</v>
       </c>
       <c r="K14" s="1648" t="n">
-        <v>39.29</v>
+        <v>40.45</v>
       </c>
       <c r="L14" s="1647" t="n">
-        <v>39.02</v>
+        <v>40.31</v>
       </c>
       <c r="M14" s="1648" t="n">
-        <v>38.96</v>
+        <v>40.31</v>
       </c>
       <c r="N14" s="143">
         <f>IF($V14="TRUETRUETRUE","(!BUY!)","HOLD")</f>
@@ -12525,25 +12525,25 @@
         </is>
       </c>
       <c r="G16" s="1646" t="n">
-        <v>235.86</v>
+        <v>242.65</v>
       </c>
       <c r="H16" s="1647" t="n">
-        <v>242.06</v>
+        <v>242.82</v>
       </c>
       <c r="I16" s="1648" t="n">
-        <v>241.03</v>
+        <v>241.26</v>
       </c>
       <c r="J16" s="1647" t="n">
-        <v>235.01</v>
+        <v>242.42</v>
       </c>
       <c r="K16" s="1648" t="n">
-        <v>234.77</v>
+        <v>242.16</v>
       </c>
       <c r="L16" s="1647" t="n">
-        <v>235.82</v>
+        <v>242.4</v>
       </c>
       <c r="M16" s="1648" t="n">
-        <v>234.7</v>
+        <v>242.31</v>
       </c>
       <c r="N16" s="227">
         <f>IF($V16="TRUETRUETRUE","(!BUY!)","HOLD")</f>
@@ -12656,25 +12656,25 @@
         </is>
       </c>
       <c r="G17" s="1646" t="n">
-        <v>184.11</v>
+        <v>203.87</v>
       </c>
       <c r="H17" s="1647" t="n">
-        <v>187.17</v>
+        <v>191.73</v>
       </c>
       <c r="I17" s="1648" t="n">
-        <v>183.51</v>
+        <v>185.09</v>
       </c>
       <c r="J17" s="1647" t="n">
-        <v>184.34</v>
+        <v>203.38</v>
       </c>
       <c r="K17" s="1648" t="n">
-        <v>186.05</v>
+        <v>202.58</v>
       </c>
       <c r="L17" s="1647" t="n">
-        <v>184.42</v>
+        <v>203.56</v>
       </c>
       <c r="M17" s="1648" t="n">
-        <v>185.74</v>
+        <v>203.14</v>
       </c>
       <c r="N17" s="147">
         <f>IF($V17="TRUETRUETRUE","(!BUY!)","HOLD")</f>
@@ -12787,25 +12787,25 @@
         </is>
       </c>
       <c r="G18" s="1646" t="n">
-        <v>416.88</v>
+        <v>435.3</v>
       </c>
       <c r="H18" s="1647" t="n">
-        <v>384.64</v>
+        <v>405.65</v>
       </c>
       <c r="I18" s="1648" t="n">
-        <v>351.05</v>
+        <v>357.63</v>
       </c>
       <c r="J18" s="1647" t="n">
-        <v>418.17</v>
+        <v>434.72</v>
       </c>
       <c r="K18" s="1648" t="n">
-        <v>419.66</v>
+        <v>434.43</v>
       </c>
       <c r="L18" s="1647" t="n">
-        <v>418.13</v>
+        <v>434.7</v>
       </c>
       <c r="M18" s="1648" t="n">
-        <v>418.24</v>
+        <v>434.74</v>
       </c>
       <c r="N18" s="147">
         <f>IF($V18="TRUETRUETRUE","(!BUY!)","HOLD")</f>
@@ -12918,25 +12918,25 @@
         </is>
       </c>
       <c r="G19" s="1646" t="n">
-        <v>164.74</v>
+        <v>180.51</v>
       </c>
       <c r="H19" s="1647" t="n">
-        <v>173.57</v>
+        <v>174.07</v>
       </c>
       <c r="I19" s="1648" t="n">
-        <v>172.09</v>
+        <v>172.55</v>
       </c>
       <c r="J19" s="1647" t="n">
-        <v>165.04</v>
+        <v>179.7</v>
       </c>
       <c r="K19" s="1648" t="n">
-        <v>166.45</v>
+        <v>178.45</v>
       </c>
       <c r="L19" s="1647" t="n">
-        <v>164.86</v>
+        <v>180.03</v>
       </c>
       <c r="M19" s="1648" t="n">
-        <v>166.2</v>
+        <v>179.14</v>
       </c>
       <c r="N19" s="143">
         <f>IF($V19="TRUETRUETRUE","(!BUY!)","HOLD")</f>
@@ -13102,25 +13102,25 @@
         </is>
       </c>
       <c r="G21" s="1706" t="n">
-        <v>80</v>
+        <v>83.09999999999999</v>
       </c>
       <c r="H21" s="1707" t="n">
-        <v>81.26000000000001</v>
+        <v>81.78</v>
       </c>
       <c r="I21" s="1708" t="n">
-        <v>85.14</v>
+        <v>83.73999999999999</v>
       </c>
       <c r="J21" s="1707" t="n">
-        <v>79.84</v>
+        <v>82.81</v>
       </c>
       <c r="K21" s="1708" t="n">
-        <v>79.56999999999999</v>
+        <v>82.8</v>
       </c>
       <c r="L21" s="1707" t="n">
-        <v>79.98999999999999</v>
+        <v>82.94</v>
       </c>
       <c r="M21" s="1708" t="n">
-        <v>79.89</v>
+        <v>82.84999999999999</v>
       </c>
       <c r="N21" s="227">
         <f>IF($V21="TRUETRUETRUE","(!BUY!)","HOLD")</f>
@@ -13232,25 +13232,25 @@
         </is>
       </c>
       <c r="G22" s="1706" t="n">
-        <v>383.89</v>
+        <v>402.51</v>
       </c>
       <c r="H22" s="1707" t="n">
-        <v>376.74</v>
+        <v>387.22</v>
       </c>
       <c r="I22" s="1708" t="n">
-        <v>364.6</v>
+        <v>366.82</v>
       </c>
       <c r="J22" s="1707" t="n">
-        <v>383.83</v>
+        <v>402</v>
       </c>
       <c r="K22" s="1708" t="n">
-        <v>385.12</v>
+        <v>401.9</v>
       </c>
       <c r="L22" s="1707" t="n">
-        <v>384.27</v>
+        <v>402.07</v>
       </c>
       <c r="M22" s="1708" t="n">
-        <v>384</v>
+        <v>401.93</v>
       </c>
       <c r="N22" s="147">
         <f>IF($V22="TRUETRUETRUE","(!BUY!)","HOLD")</f>
@@ -13362,25 +13362,25 @@
         </is>
       </c>
       <c r="G23" s="1706" t="n">
-        <v>101.49</v>
+        <v>105.39</v>
       </c>
       <c r="H23" s="1714" t="n">
-        <v>97.39</v>
+        <v>100.76</v>
       </c>
       <c r="I23" s="1715" t="n">
-        <v>91.06999999999999</v>
+        <v>91.81999999999999</v>
       </c>
       <c r="J23" s="1716" t="n">
-        <v>101.37</v>
+        <v>105.44</v>
       </c>
       <c r="K23" s="1708" t="n">
-        <v>101.44</v>
+        <v>105.57</v>
       </c>
       <c r="L23" s="1707" t="n">
-        <v>101.49</v>
+        <v>105.3</v>
       </c>
       <c r="M23" s="1708" t="n">
-        <v>101.36</v>
+        <v>105.62</v>
       </c>
       <c r="N23" s="147">
         <f>IF($V23="TRUETRUETRUE","(!BUY!)","HOLD")</f>
@@ -13490,25 +13490,25 @@
         </is>
       </c>
       <c r="G24" s="1706" t="n">
-        <v>73.04000000000001</v>
+        <v>72.44</v>
       </c>
       <c r="H24" s="1707" t="n">
-        <v>73.55</v>
+        <v>73.11</v>
       </c>
       <c r="I24" s="1708" t="n">
-        <v>72.87</v>
+        <v>72.66</v>
       </c>
       <c r="J24" s="1707" t="n">
-        <v>72.98</v>
+        <v>72.38</v>
       </c>
       <c r="K24" s="1708" t="n">
-        <v>72.7</v>
+        <v>72.67</v>
       </c>
       <c r="L24" s="1707" t="n">
-        <v>73.06</v>
+        <v>72.40000000000001</v>
       </c>
       <c r="M24" s="1708" t="n">
-        <v>73.01000000000001</v>
+        <v>72.38</v>
       </c>
       <c r="N24" s="147">
         <f>IF($V24="TRUETRUETRUE","(!BUY!)","HOLD")</f>
@@ -13684,25 +13684,25 @@
         </is>
       </c>
       <c r="G26" s="1646" t="n">
-        <v>48.95</v>
+        <v>48.81</v>
       </c>
       <c r="H26" s="1728" t="n">
+        <v>48.73</v>
+      </c>
+      <c r="I26" s="1729" t="n">
+        <v>48.43</v>
+      </c>
+      <c r="J26" s="1728" t="n">
         <v>48.77</v>
       </c>
-      <c r="I26" s="1729" t="n">
-        <v>48.52</v>
-      </c>
-      <c r="J26" s="1728" t="n">
-        <v>48.91</v>
-      </c>
       <c r="K26" s="1729" t="n">
-        <v>48.7</v>
+        <v>48.88</v>
       </c>
       <c r="L26" s="1730" t="n">
-        <v>48.94</v>
+        <v>48.77</v>
       </c>
       <c r="M26" s="1731" t="n">
-        <v>48.92</v>
+        <v>48.77</v>
       </c>
       <c r="N26" s="147">
         <f>IF($V26="TRUETRUETRUE","(!BUY!)","HOLD")</f>
@@ -13813,25 +13813,25 @@
         </is>
       </c>
       <c r="G27" s="1646" t="n">
-        <v>54.28</v>
+        <v>55.5</v>
       </c>
       <c r="H27" s="1647" t="n">
-        <v>55.5</v>
+        <v>55.94</v>
       </c>
       <c r="I27" s="1648" t="n">
-        <v>52.71</v>
+        <v>53.13</v>
       </c>
       <c r="J27" s="1647" t="n">
-        <v>54.12</v>
+        <v>55.44</v>
       </c>
       <c r="K27" s="1648" t="n">
-        <v>54.63</v>
+        <v>55.52</v>
       </c>
       <c r="L27" s="1647" t="n">
-        <v>54.25</v>
+        <v>55.45</v>
       </c>
       <c r="M27" s="1648" t="n">
-        <v>54.16</v>
+        <v>55.44</v>
       </c>
       <c r="N27" s="147">
         <f>IF($V27="TRUETRUETRUE","(!BUY!)","HOLD")</f>
@@ -13943,25 +13943,25 @@
         </is>
       </c>
       <c r="G28" s="1646" t="n">
-        <v>207.18</v>
+        <v>218.02</v>
       </c>
       <c r="H28" s="1647" t="n">
-        <v>203.77</v>
+        <v>209.3</v>
       </c>
       <c r="I28" s="1648" t="n">
-        <v>198.59</v>
+        <v>199.58</v>
       </c>
       <c r="J28" s="1647" t="n">
-        <v>207.13</v>
+        <v>217.72</v>
       </c>
       <c r="K28" s="1648" t="n">
-        <v>207.87</v>
+        <v>217.05</v>
       </c>
       <c r="L28" s="1647" t="n">
-        <v>207.39</v>
+        <v>217.76</v>
       </c>
       <c r="M28" s="1648" t="n">
-        <v>207.23</v>
+        <v>217.69</v>
       </c>
       <c r="N28" s="147">
         <f>IF($V28="TRUETRUETRUE","(!BUY!)","HOLD")</f>
@@ -14071,25 +14071,25 @@
         </is>
       </c>
       <c r="G29" s="1646" t="n">
-        <v>141.32</v>
+        <v>140.63</v>
       </c>
       <c r="H29" s="1647" t="n">
-        <v>147.25</v>
+        <v>145.74</v>
       </c>
       <c r="I29" s="1648" t="n">
-        <v>150.49</v>
+        <v>148.25</v>
       </c>
       <c r="J29" s="1647" t="n">
-        <v>141.18</v>
+        <v>140.97</v>
       </c>
       <c r="K29" s="1648" t="n">
-        <v>140.53</v>
+        <v>141.98</v>
       </c>
       <c r="L29" s="1647" t="n">
-        <v>141.58</v>
+        <v>140.78</v>
       </c>
       <c r="M29" s="1648" t="n">
-        <v>140.7</v>
+        <v>140.82</v>
       </c>
       <c r="N29" s="143">
         <f>IF($V29="TRUETRUETRUE","(!BUY!)","HOLD")</f>
@@ -14201,25 +14201,25 @@
         </is>
       </c>
       <c r="G30" s="1646" t="n">
-        <v>71.95999999999999</v>
+        <v>83.34</v>
       </c>
       <c r="H30" s="1647" t="n">
-        <v>71.63</v>
+        <v>74.68000000000001</v>
       </c>
       <c r="I30" s="1648" t="n">
-        <v>72.2</v>
+        <v>72.47</v>
       </c>
       <c r="J30" s="1647" t="n">
-        <v>72.01000000000001</v>
+        <v>83.31</v>
       </c>
       <c r="K30" s="1648" t="n">
-        <v>72.54000000000001</v>
+        <v>81.28</v>
       </c>
       <c r="L30" s="1647" t="n">
-        <v>72</v>
+        <v>83.23</v>
       </c>
       <c r="M30" s="1648" t="n">
-        <v>72.56999999999999</v>
+        <v>82.18000000000001</v>
       </c>
       <c r="N30" s="147">
         <f>IF($V30="TRUETRUETRUE","(!BUY!)","HOLD")</f>

</xml_diff>